<commit_message>
Cheque window - some fixes
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -923,9 +923,15 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1217,23 +1223,23 @@
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" style="29" customWidth="1"/>
     <col min="8" max="8" width="6" style="8" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="0.33203125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="8"/>
+    <col min="9" max="9" width="3.7109375" style="8" customWidth="1"/>
+    <col min="10" max="10" width="0.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1256,7 +1262,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1287,7 +1293,7 @@
         <v>108.4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
@@ -1322,7 +1328,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>21</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
@@ -1398,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="11">
         <f t="shared" si="1"/>
@@ -1421,7 +1427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="11">
         <f t="shared" si="1"/>
@@ -1445,7 +1451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
@@ -1469,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
@@ -1494,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="11">
         <f t="shared" si="1"/>
@@ -1565,7 +1571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="11">
         <f t="shared" si="1"/>
@@ -1589,7 +1595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="11">
         <f t="shared" si="1"/>
@@ -1607,7 +1613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="11">
         <f t="shared" si="1"/>
@@ -1625,7 +1631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
@@ -1653,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>21</v>
       </c>
@@ -1697,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="11">
         <f t="shared" si="1"/>
@@ -1715,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
@@ -1759,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="11">
         <f t="shared" si="1"/>
@@ -1783,7 +1789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="11">
         <f t="shared" si="1"/>
@@ -1799,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="11">
         <f t="shared" si="1"/>
@@ -1815,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="11">
         <f t="shared" si="1"/>
@@ -1837,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="11">
         <f t="shared" si="1"/>
@@ -1859,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="11">
         <f t="shared" si="1"/>
@@ -1881,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="11">
         <f t="shared" si="1"/>
@@ -1900,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="11">
         <f t="shared" si="1"/>
@@ -1919,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="11">
         <f t="shared" si="1"/>
@@ -1939,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="11">
         <f t="shared" si="1"/>
@@ -1956,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="11">
         <f t="shared" si="1"/>
@@ -1970,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="11">
         <f t="shared" si="1"/>
@@ -1984,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="11">
         <f t="shared" si="1"/>
@@ -1998,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="11">
         <f t="shared" si="1"/>
@@ -2012,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="11">
         <f t="shared" si="1"/>
@@ -2028,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="11">
         <f t="shared" si="1"/>
@@ -2042,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="11">
         <f t="shared" si="1"/>
@@ -2056,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="11">
         <f t="shared" si="1"/>
@@ -2070,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="11">
         <f t="shared" si="1"/>
@@ -2084,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="11">
         <f t="shared" si="1"/>
@@ -2097,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="11">
         <f t="shared" si="1"/>
@@ -2111,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="11">
         <f t="shared" si="1"/>
@@ -2125,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="11">
         <f t="shared" si="1"/>
@@ -2139,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="11">
         <f t="shared" si="1"/>
@@ -2153,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="11">
         <f t="shared" si="1"/>
@@ -2167,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="11">
         <f t="shared" si="1"/>
@@ -2181,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
       <c r="B49" s="11">
         <f t="shared" si="1"/>
@@ -2195,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
       <c r="B50" s="11">
         <f t="shared" si="1"/>
@@ -2209,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="11">
         <f t="shared" si="1"/>
@@ -2223,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="16"/>
       <c r="B52" s="11">
         <f t="shared" si="1"/>
@@ -2247,26 +2253,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.77734375" style="34" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" style="34" customWidth="1"/>
     <col min="2" max="2" width="10" style="36" customWidth="1"/>
-    <col min="3" max="3" width="2.44140625" customWidth="1"/>
-    <col min="4" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="1.44140625" customWidth="1"/>
-    <col min="8" max="8" width="24.109375" style="37" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="37" customWidth="1"/>
     <col min="10" max="10" width="12" style="37" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" style="37" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>2</v>
       </c>
@@ -2292,7 +2298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>98</v>
       </c>
@@ -2301,14 +2307,14 @@
       </c>
       <c r="D2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43171</v>
+        <v>43174</v>
       </c>
       <c r="E2" s="27">
         <v>43282</v>
       </c>
       <c r="F2" s="25">
         <f ca="1">E2-D2</f>
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H2" s="25">
         <f>SUM(B2:B141)</f>
@@ -2316,10 +2322,10 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">F2-H2</f>
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>99</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>100</v>
       </c>
@@ -2359,7 +2365,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>101</v>
       </c>
@@ -2379,7 +2385,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>144</v>
       </c>
@@ -2399,7 +2405,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>143</v>
       </c>
@@ -2416,21 +2422,21 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>102</v>
       </c>
       <c r="B8" s="42">
         <v>0</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="45" t="s">
         <v>115</v>
       </c>
       <c r="J8" s="39" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>103</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>104</v>
       </c>
@@ -2452,7 +2458,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>105</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>106</v>
       </c>
@@ -2471,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>107</v>
       </c>
@@ -2479,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
         <v>108</v>
       </c>
@@ -2487,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>145</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>109</v>
       </c>
@@ -2503,15 +2509,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="47">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>60</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>118</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>15</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>22</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>123</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>129</v>
       </c>
@@ -2559,7 +2565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>135</v>
       </c>
@@ -2567,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>136</v>
       </c>
@@ -2575,7 +2581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
         <v>75</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>74</v>
       </c>
@@ -2591,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>68</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>138</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
         <v>86</v>
       </c>
@@ -2615,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
         <v>90</v>
       </c>
@@ -2623,7 +2629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
         <v>91</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
         <v>94</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
         <v>85</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
         <v>81</v>
       </c>
@@ -2655,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
         <v>73</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
         <v>83</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
         <v>139</v>
       </c>
@@ -2679,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="34" t="s">
         <v>163</v>
       </c>
@@ -2697,18 +2703,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" style="32" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" style="32" customWidth="1"/>
-    <col min="3" max="4" width="63.109375" style="32" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="32" customWidth="1"/>
+    <col min="3" max="4" width="63.140625" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>76</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>165</v>
       </c>
@@ -2733,7 +2739,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>167</v>
       </c>
@@ -2747,7 +2753,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>168</v>
       </c>
@@ -2758,7 +2764,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>169</v>
       </c>
@@ -2769,7 +2775,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
         <v>88</v>
       </c>
@@ -2777,7 +2783,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>141</v>
       </c>
@@ -2791,7 +2797,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>142</v>
       </c>
@@ -2805,7 +2811,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="32" t="s">
         <v>95</v>
       </c>
@@ -2813,42 +2819,42 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="32" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="32" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="32" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="32" t="s">
         <v>160</v>
       </c>
@@ -2866,13 +2872,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="78.6640625" style="44" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>146</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>148</v>
       </c>
@@ -2888,7 +2894,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>151</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>151</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>154</v>
       </c>
@@ -2920,7 +2926,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>154</v>
       </c>
@@ -2928,7 +2934,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>157</v>
       </c>
@@ -2936,7 +2942,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>158</v>
       </c>
@@ -2944,7 +2950,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>149</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>149</v>
       </c>
@@ -2960,7 +2966,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>158</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
Transactions page settings. DB
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="176">
   <si>
     <t>№</t>
   </si>
@@ -548,6 +548,12 @@
   </si>
   <si>
     <t>Events: "Create transaction" menu item -&gt; show record details</t>
+  </si>
+  <si>
+    <t>Refactoring: create separate control for period selector</t>
+  </si>
+  <si>
+    <t>Refactoring: create separate control for data filter</t>
   </si>
 </sst>
 </file>
@@ -2279,11 +2285,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2329,22 +2335,22 @@
       <c r="B2" s="45"/>
       <c r="D2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43176</v>
+        <v>43177</v>
       </c>
       <c r="E2" s="27">
         <v>43282</v>
       </c>
       <c r="F2" s="25">
         <f ca="1">E2-D2</f>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H2" s="25">
-        <f>SUM(B3:B169)</f>
-        <v>130</v>
+        <f>SUM(B3:B171)</f>
+        <v>131</v>
       </c>
       <c r="I2" s="25">
         <f ca="1">F2-H2</f>
-        <v>-24</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2497,11 +2503,11 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="34">
-        <v>1</v>
+      <c r="B21" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2546,175 +2552,175 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="B27" s="34">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B28" s="34">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B29" s="34">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B30" s="34">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="33" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B31" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B32" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B33" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="33" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B34" s="34">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
       <c r="B35" s="34">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="33" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="B36" s="34">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
-        <v>162</v>
+        <v>15</v>
       </c>
       <c r="B37" s="34">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
-        <v>157</v>
+        <v>22</v>
       </c>
       <c r="B38" s="34">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="33" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B39" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B40" s="34">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B41" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="33" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B42" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B44" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B45" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B46" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B47" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B48" s="34">
         <v>1</v>
@@ -2722,103 +2728,103 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B49" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B50" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B51" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
-        <v>110</v>
+        <v>166</v>
       </c>
       <c r="B52" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="33" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="B53" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="33" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B54" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="34">
+      <c r="B57" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="37" t="s">
+      <c r="B58" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="B58" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B59" s="34">
-        <v>1</v>
+      <c r="B59" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="33" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B60" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="33" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="B61" s="34">
         <v>1</v>
@@ -2826,15 +2832,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B62" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="B63" s="34">
         <v>1</v>
@@ -2842,7 +2848,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B64" s="34">
         <v>1</v>
@@ -2850,7 +2856,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B65" s="34">
         <v>1</v>
@@ -2858,17 +2864,33 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="33" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="B66" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B67" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="B67" s="34">
+      <c r="B69" s="34">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Transactions page filter. In development
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -2288,8 +2288,8 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2335,14 +2335,14 @@
       <c r="B2" s="45"/>
       <c r="D2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43177</v>
+        <v>43178</v>
       </c>
       <c r="E2" s="27">
         <v>43282</v>
       </c>
       <c r="F2" s="25">
         <f ca="1">E2-D2</f>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="25">
         <f>SUM(B3:B171)</f>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="I2" s="25">
         <f ca="1">F2-H2</f>
-        <v>-26</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Improve performance on main view loading
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -442,9 +442,6 @@
     <t>Вынести opacity в отдельный файл стилей</t>
   </si>
   <si>
-    <t>Replace OrderBy into the service</t>
-  </si>
-  <si>
     <t>Создать свои стили для всех компонентов (не использовать MetroStyle/MaterialDesign)</t>
   </si>
   <si>
@@ -563,6 +560,9 @@
   </si>
   <si>
     <t>Data filter control -&gt; category tree context menu (expand all, collapse all, select all, upselect all, select branch, unselect branch)</t>
+  </si>
+  <si>
+    <t>Replace OrderBy into the service in the entity selections</t>
   </si>
 </sst>
 </file>
@@ -861,7 +861,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -972,6 +972,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2297,8 +2298,8 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <pane ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2355,11 +2356,11 @@
       </c>
       <c r="H2" s="25">
         <f>SUM(B3:B171)</f>
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I2" s="25">
         <f ca="1">F2-H2</f>
-        <v>-37</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2489,7 +2490,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" s="38">
         <v>0</v>
@@ -2497,7 +2498,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="38">
         <v>0</v>
@@ -2505,7 +2506,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="38">
         <v>0</v>
@@ -2513,7 +2514,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="38">
         <v>0</v>
@@ -2521,7 +2522,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" s="38">
         <v>0</v>
@@ -2529,7 +2530,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" s="38">
         <v>0</v>
@@ -2537,7 +2538,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B24" s="38">
         <v>0</v>
@@ -2545,7 +2546,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" s="34">
         <v>1</v>
@@ -2553,7 +2554,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B26" s="38">
         <v>0</v>
@@ -2561,23 +2562,23 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B27" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="B28" s="34">
-        <v>1</v>
+      <c r="A28" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B29" s="34">
         <v>7</v>
@@ -2585,7 +2586,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30" s="34">
         <v>7</v>
@@ -2593,7 +2594,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B31" s="34">
         <v>3</v>
@@ -2601,7 +2602,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B32" s="34">
         <v>3</v>
@@ -2609,7 +2610,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B33" s="34">
         <v>2</v>
@@ -2617,7 +2618,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B34" s="34">
         <v>2</v>
@@ -2625,7 +2626,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B35" s="34">
         <v>1</v>
@@ -2633,7 +2634,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B36" s="34">
         <v>4</v>
@@ -2657,7 +2658,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" s="34">
         <v>2</v>
@@ -2665,7 +2666,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B40" s="34">
         <v>7</v>
@@ -2673,7 +2674,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B41" s="34">
         <v>1</v>
@@ -2681,7 +2682,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B42" s="34">
         <v>4</v>
@@ -2689,7 +2690,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="34">
         <v>3</v>
@@ -2697,7 +2698,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B44" s="34">
         <v>1</v>
@@ -2705,7 +2706,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45" s="34">
         <v>2</v>
@@ -2713,7 +2714,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B46" s="34">
         <v>2</v>
@@ -2721,7 +2722,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B47" s="34">
         <v>3</v>
@@ -2729,7 +2730,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B48" s="34">
         <v>1</v>
@@ -2737,7 +2738,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B49" s="34">
         <v>2</v>
@@ -2745,7 +2746,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B50" s="34">
         <v>1</v>
@@ -2753,7 +2754,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B51" s="34">
         <v>1</v>
@@ -2761,7 +2762,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B52" s="34">
         <v>1</v>
@@ -2769,7 +2770,7 @@
     </row>
     <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B53" s="34">
         <v>3</v>
@@ -2849,7 +2850,7 @@
     </row>
     <row r="63" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B63" s="34">
         <v>1</v>
@@ -2897,7 +2898,7 @@
     </row>
     <row r="69" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B69" s="34">
         <v>1</v>
@@ -2905,7 +2906,7 @@
     </row>
     <row r="70" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B70" s="34">
         <v>2</v>
@@ -3079,7 +3080,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3181,7 +3182,7 @@
         <v>133</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3189,15 +3190,15 @@
         <v>124</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="46" t="s">
         <v>176</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calendar page (in development)
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EDA5DAD4-8FFC-4801-BEE3-4C551E842357}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="1" r:id="rId1"/>
@@ -571,7 +572,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -969,13 +970,13 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1261,7 +1262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:L52"/>
   <sheetViews>
@@ -2297,12 +2298,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2321,10 +2322,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>56</v>
       </c>
       <c r="D1" s="26" t="s">
@@ -2344,26 +2345,26 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
       <c r="D2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43189</v>
+        <v>43191</v>
       </c>
       <c r="E2" s="27">
         <v>43282</v>
       </c>
       <c r="F2" s="25">
         <f ca="1">E2-D2</f>
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H2" s="25">
         <f>SUM(B3:B171)</f>
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I2" s="25">
         <f ca="1">F2-H2</f>
-        <v>-31</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2584,7 +2585,7 @@
         <v>148</v>
       </c>
       <c r="B29" s="34">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2600,7 +2601,7 @@
         <v>151</v>
       </c>
       <c r="B31" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2616,7 +2617,7 @@
         <v>150</v>
       </c>
       <c r="B33" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2942,7 +2943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3090,7 +3091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3208,10 +3209,10 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="44" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calendar page: show total income/expence for day
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3295C7A7-68DB-4B80-A784-335518EA248B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3B259222-55B1-4377-9FAC-5F96C65F477F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,7 @@
     <sheet name="Estimate" sheetId="2" r:id="rId2"/>
     <sheet name="Bugs" sheetId="4" r:id="rId3"/>
     <sheet name="Refactoring" sheetId="5" r:id="rId4"/>
+    <sheet name="Help" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plans!$A$1:$E$52</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="191">
   <si>
     <t>№</t>
   </si>
@@ -245,9 +246,6 @@
     <t>All buttons ToggleButton -&gt; change icon when unckecked and change tooltip</t>
   </si>
   <si>
-    <t>Ограничения на строки (DetailsView)</t>
-  </si>
-  <si>
     <t>Обработчики delete exceptions</t>
   </si>
   <si>
@@ -269,9 +267,6 @@
     <t>User local settings -&gt; main menu shown</t>
   </si>
   <si>
-    <t>Categories page -&gt; expand all/collapse all</t>
-  </si>
-  <si>
     <t>Если приложение падает, отправлять мейл. Хранить ошибки в бд</t>
   </si>
   <si>
@@ -296,21 +291,12 @@
     <t>User settings - autofill description from selected category</t>
   </si>
   <si>
-    <t>Storages page -&gt; double click -&gt; edit</t>
-  </si>
-  <si>
-    <t>Storages page -&gt; drug/drop</t>
-  </si>
-  <si>
     <t>Debts page. Model. Binding.</t>
   </si>
   <si>
     <t>Replace all additional fields from models to view models</t>
   </si>
   <si>
-    <t>For every new entity fill default requires foreign key values</t>
-  </si>
-  <si>
     <t>Check details view on enums</t>
   </si>
   <si>
@@ -329,69 +315,18 @@
     <t>RepayDebtEventDetailsView</t>
   </si>
   <si>
-    <t>PlanningPage -&gt; Limits list + LimitDetailsView</t>
-  </si>
-  <si>
-    <t>Refactoring: base details view</t>
-  </si>
-  <si>
-    <t>Refactoring: models &amp; view models</t>
-  </si>
-  <si>
-    <t>Refactoring: services (onAdd, onEdit, onDelete methods)</t>
-  </si>
-  <si>
-    <t>Refactoring: Commission in entities(models) to separate entity</t>
-  </si>
-  <si>
-    <t>Refactoring: default command implementations</t>
-  </si>
-  <si>
-    <t>Refactoring: Check details view on enums</t>
-  </si>
-  <si>
-    <t>Refactoring: List view -&gt; enum value converter (instead of combobox)</t>
-  </si>
-  <si>
-    <t>Refactoring: Придумать заполнение Combobox nullable ids</t>
-  </si>
-  <si>
     <t>Add family</t>
   </si>
   <si>
-    <t>Settings page: general data</t>
-  </si>
-  <si>
-    <t>Settings page: theme and language</t>
-  </si>
-  <si>
     <t>Remained time</t>
   </si>
   <si>
     <t>Expander size: fix columns size</t>
   </si>
   <si>
-    <t>Events: "apply now" menu item</t>
-  </si>
-  <si>
     <t>Add targets</t>
   </si>
   <si>
-    <t>Debts list -&gt; foreground green/red</t>
-  </si>
-  <si>
-    <t>Money transfer events list -&gt; foreground red if commission exists</t>
-  </si>
-  <si>
-    <t>Refactoring: page options and reload requirements</t>
-  </si>
-  <si>
-    <t>Refactoring: custom controls (category selection dialog, comission control, currency exchange rate selector)</t>
-  </si>
-  <si>
-    <t>Refactoring: see all details views on margin, result value, perfect visual style</t>
-  </si>
-  <si>
     <t>Requires refactoring</t>
   </si>
   <si>
@@ -443,136 +378,229 @@
     <t>Создать свои стили для всех компонентов (не использовать MetroStyle/MaterialDesign)</t>
   </si>
   <si>
-    <t>Transactions page. Records list</t>
-  </si>
-  <si>
-    <t>Transactions page. Record details</t>
-  </si>
-  <si>
-    <t>Transactions page. Filter</t>
-  </si>
-  <si>
-    <t>Transactions page. Show for period</t>
-  </si>
-  <si>
-    <t>Transactions page. Show planned events</t>
-  </si>
-  <si>
-    <t>Transactions page. Show money transfers in list</t>
-  </si>
-  <si>
-    <t>Transactions page. Context menu for planned</t>
-  </si>
-  <si>
-    <t>Transactions page. Add cheque</t>
-  </si>
-  <si>
-    <t>Transactions page. Save filter to DB</t>
-  </si>
-  <si>
-    <t>CalendarDataBuilder. Limits</t>
-  </si>
-  <si>
-    <t>CalendarDataBuilder. Day data</t>
-  </si>
-  <si>
-    <t>Calendar page. Show for period</t>
-  </si>
-  <si>
-    <t>Calendar page. Calendar day control</t>
-  </si>
-  <si>
-    <t>Calendar page. Base view</t>
-  </si>
-  <si>
-    <t>Calendar page. Open list/details on double click</t>
-  </si>
-  <si>
-    <t>Reports page. Pie chart</t>
-  </si>
-  <si>
-    <t>Reports page. Table</t>
-  </si>
-  <si>
-    <t>Reports page. Bar chart</t>
-  </si>
-  <si>
-    <t>Reports page. Filter</t>
-  </si>
-  <si>
-    <t>Reports page. Data builder</t>
-  </si>
-  <si>
-    <t>Reports page. Base view</t>
-  </si>
-  <si>
-    <t>Reports page. Show for period</t>
-  </si>
-  <si>
-    <t>Dashboard. Base view</t>
-  </si>
-  <si>
-    <t>Dashboard. Today transactions</t>
-  </si>
-  <si>
-    <t>Dashboard. Balance summary</t>
-  </si>
-  <si>
-    <t>Dashboard. Events for confirmation DB</t>
-  </si>
-  <si>
-    <t>Dashboard. Events for confirmation View</t>
-  </si>
-  <si>
-    <t>Dashboard. Events to be executed today DB</t>
-  </si>
-  <si>
-    <t>Dashboard. Events to be executed today View</t>
-  </si>
-  <si>
-    <t>Dashboard. Alerts: exceeded limit, debt should be repayed…</t>
-  </si>
-  <si>
     <t>For every new entity fill default required foreign key values</t>
   </si>
   <si>
-    <t>Events: "Create transaction" menu item -&gt; show record details</t>
-  </si>
-  <si>
-    <t>Refactoring: create separate control for period selector</t>
-  </si>
-  <si>
-    <t>Refactoring: create separate control for data filter</t>
-  </si>
-  <si>
     <t>Perfomance</t>
   </si>
   <si>
     <t>Replace all data loading in pages into the loaded event instead of constructor</t>
   </si>
   <si>
-    <t>Data filter control -&gt; category tree context menu (expand all, collapse all, select all, upselect all, select branch, unselect branch)</t>
-  </si>
-  <si>
     <t>Replace OrderBy into the service in the entity selections</t>
   </si>
   <si>
-    <t>Transactions Page: show/hide planned transactions</t>
-  </si>
-  <si>
     <t>Update limits on record/money transfer is added</t>
   </si>
   <si>
-    <t>Calendar page. Settings</t>
-  </si>
-  <si>
-    <t>Calendar page. Save settings to DB</t>
-  </si>
-  <si>
-    <t>Event services</t>
-  </si>
-  <si>
-    <t>Make generic Currency exchange rage updating</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Feature(G)</t>
+  </si>
+  <si>
+    <t>Custom controls (category selection dialog, comission control, currency exchange rate selector)</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Details view</t>
+  </si>
+  <si>
+    <t>PlanningPage</t>
+  </si>
+  <si>
+    <t>Limits list + LimitDetailsView</t>
+  </si>
+  <si>
+    <t>Records list</t>
+  </si>
+  <si>
+    <t>Transactions page</t>
+  </si>
+  <si>
+    <t>Record details</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Save filter to DB</t>
+  </si>
+  <si>
+    <t>Show for period</t>
+  </si>
+  <si>
+    <t>Show planned events</t>
+  </si>
+  <si>
+    <t>Show money transfers in list</t>
+  </si>
+  <si>
+    <t>Context menu for planned</t>
+  </si>
+  <si>
+    <t>Add cheque</t>
+  </si>
+  <si>
+    <t>Create separate control for period selector</t>
+  </si>
+  <si>
+    <t>Create separate control for data filter</t>
+  </si>
+  <si>
+    <t>Day data</t>
+  </si>
+  <si>
+    <t>Limits</t>
+  </si>
+  <si>
+    <t>CalendarDataBuilder</t>
+  </si>
+  <si>
+    <t>Page options and reload requirements</t>
+  </si>
+  <si>
+    <t>Base details view</t>
+  </si>
+  <si>
+    <t>Models &amp; view models</t>
+  </si>
+  <si>
+    <t>Services (onAdd, onEdit, onDelete methods)</t>
+  </si>
+  <si>
+    <t>Default command implementations</t>
+  </si>
+  <si>
+    <t>See all details views on margin, result value, perfect visual style</t>
+  </si>
+  <si>
+    <t>Base view</t>
+  </si>
+  <si>
+    <t>Calendar page</t>
+  </si>
+  <si>
+    <t>Calendar day control</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Save settings to DB</t>
+  </si>
+  <si>
+    <t>Open list/details on double click</t>
+  </si>
+  <si>
+    <t>Reports page</t>
+  </si>
+  <si>
+    <t>Pie chart</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Bar chart</t>
+  </si>
+  <si>
+    <t>Data builder</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Events for confirmation DB</t>
+  </si>
+  <si>
+    <t>Events for confirmation View</t>
+  </si>
+  <si>
+    <t>Events to be executed today DB</t>
+  </si>
+  <si>
+    <t>Events to be executed today View</t>
+  </si>
+  <si>
+    <t>Today transactions</t>
+  </si>
+  <si>
+    <t>Balance summary</t>
+  </si>
+  <si>
+    <t>Alerts: exceeded limit, debt should be repayed…</t>
+  </si>
+  <si>
+    <t>General data</t>
+  </si>
+  <si>
+    <t>Settings page</t>
+  </si>
+  <si>
+    <t>Theme and language</t>
+  </si>
+  <si>
+    <t>double click -&gt; edit</t>
+  </si>
+  <si>
+    <t>Storages page</t>
+  </si>
+  <si>
+    <t>drug/drop</t>
+  </si>
+  <si>
+    <t>Summary for every group</t>
+  </si>
+  <si>
+    <t>"apply now" menu item</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>"Create transaction" menu item -&gt; show record details</t>
+  </si>
+  <si>
+    <t>Data filter control</t>
+  </si>
+  <si>
+    <t>Category tree context menu (expand all, collapse all, select all, upselect all, select branch, unselect branch)</t>
+  </si>
+  <si>
+    <t>Transactions Page</t>
+  </si>
+  <si>
+    <t>Show/hide planned transactions</t>
+  </si>
+  <si>
+    <t>Debts list</t>
+  </si>
+  <si>
+    <t>Foreground green/red</t>
+  </si>
+  <si>
+    <t>Foreground red if commission exists</t>
+  </si>
+  <si>
+    <t>Money transfer events list</t>
+  </si>
+  <si>
+    <t>Expand all/collapse all</t>
+  </si>
+  <si>
+    <t>Categories page</t>
+  </si>
+  <si>
+    <t>Ограничения на строки</t>
   </si>
 </sst>
 </file>
@@ -871,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -982,6 +1010,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2009,7 +2050,7 @@
       <c r="D32" s="13"/>
       <c r="E32" s="14"/>
       <c r="G32" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J32" s="8">
         <f t="shared" si="0"/>
@@ -2305,695 +2346,963 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="10" style="34" customWidth="1"/>
-    <col min="3" max="3" width="2.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="7" width="1.44140625" customWidth="1"/>
-    <col min="8" max="8" width="24.109375" style="35" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="35" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="35" customWidth="1"/>
-    <col min="11" max="11" width="26.5546875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="50" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="10" style="34" customWidth="1"/>
+    <col min="5" max="5" width="2.21875" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="9" max="9" width="1.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.109375" style="35" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" style="35" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="26.5546875" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:11" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="D1" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="J1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
+      <c r="K1" s="36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="48"/>
       <c r="B2" s="46"/>
-      <c r="D2" s="27">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43197</v>
-      </c>
-      <c r="E2" s="27">
+        <v>43198</v>
+      </c>
+      <c r="G2" s="27">
         <v>43282</v>
       </c>
-      <c r="F2" s="25">
-        <f ca="1">E2-D2</f>
-        <v>85</v>
-      </c>
       <c r="H2" s="25">
-        <f>SUM(B3:B171)</f>
+        <f ca="1">G2-F2</f>
+        <v>84</v>
+      </c>
+      <c r="J2" s="25">
+        <f>SUM(D3:D171)</f>
+        <v>120</v>
+      </c>
+      <c r="K2" s="25">
+        <f ca="1">H2-J2</f>
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="38">
+        <v>0</v>
+      </c>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="49"/>
+      <c r="C8" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="49"/>
+      <c r="C14" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="49"/>
+      <c r="C15" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="49"/>
+      <c r="B18" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="49"/>
+      <c r="B20" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="49"/>
+      <c r="B22" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="49"/>
+      <c r="B24" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="49"/>
+      <c r="C27" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="49"/>
+      <c r="C28" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+      <c r="B31" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D34" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="D50" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="49"/>
+      <c r="C58" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="49"/>
+      <c r="C59" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="D62" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="25">
-        <f ca="1">F2-H2</f>
-        <v>-31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="38">
-        <v>0</v>
-      </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="34">
+      <c r="D63" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C64" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B65" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D65" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B66" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D66" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B67" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="D67" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B68" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="C68" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B69" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="D69" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B70" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="D70" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="34">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B71" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="D71" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C72" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="34">
+      <c r="D72" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="B20" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
-        <v>143</v>
-      </c>
-      <c r="B24" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="34">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D73" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
-        <v>145</v>
-      </c>
-      <c r="B26" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="B27" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="B29" s="34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B30" s="34">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="B31" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="37" t="s">
-        <v>149</v>
-      </c>
-      <c r="B32" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="B33" s="34">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B74" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="B34" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="B35" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="34">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="34">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="B40" s="34">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B42" s="34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B43" s="34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="B44" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="B46" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="B47" s="34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="B48" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B49" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="B50" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="B51" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B52" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B53" s="34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B56" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="B63" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B64" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B65" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="B67" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="B68" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B69" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="B70" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="B71" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="B72" s="34">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B67D7FCE-5958-4F9D-8EF5-7923E0C7736A}">
+          <x14:formula1>
+            <xm:f>Help!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.5546875" style="32" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="47.5546875" style="32" customWidth="1"/>
     <col min="3" max="4" width="63.109375" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>70</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="26" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="32" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C2" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3001,94 +3310,54 @@
         <v>71</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="32" t="s">
-        <v>86</v>
-      </c>
       <c r="D5" s="32" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>116</v>
-      </c>
       <c r="B7" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>117</v>
-      </c>
       <c r="B8" s="32" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
-        <v>94</v>
-      </c>
       <c r="C9" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C14" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3098,7 +3367,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -3112,122 +3381,157 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="44" t="s">
-        <v>172</v>
+        <v>117</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>181</v>
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266E4AE6-A920-4399-9106-F6BA9167C0EC}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calendar day: show transaction list
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3B259222-55B1-4377-9FAC-5F96C65F477F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A1852856-7329-4A9A-913B-3EF9E2B5C72C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="196">
   <si>
     <t>№</t>
   </si>
@@ -601,6 +601,21 @@
   </si>
   <si>
     <t>Ограничения на строки</t>
+  </si>
+  <si>
+    <t>Cell height in settings</t>
+  </si>
+  <si>
+    <t>When change income/expence resultat amount isn't changed</t>
+  </si>
+  <si>
+    <t>Description change doesn't make form dirty</t>
+  </si>
+  <si>
+    <t>Scroll doen't work on tree view</t>
+  </si>
+  <si>
+    <t>Show dots when many transactions</t>
   </si>
 </sst>
 </file>
@@ -2346,11 +2361,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,11 +2432,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D171)</f>
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-36</v>
+        <v>-41</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3135,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B65" s="50" t="s">
         <v>189</v>
       </c>
@@ -3146,7 +3161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B66" s="50" t="s">
         <v>127</v>
       </c>
@@ -3157,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B67" s="50" t="s">
         <v>174</v>
       </c>
@@ -3168,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B68" s="50" t="s">
         <v>178</v>
       </c>
@@ -3179,7 +3194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B69" s="50" t="s">
         <v>178</v>
       </c>
@@ -3190,7 +3205,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="50" t="s">
+        <v>123</v>
+      </c>
       <c r="B70" s="50" t="s">
         <v>180</v>
       </c>
@@ -3201,7 +3219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B71" s="50" t="s">
         <v>182</v>
       </c>
@@ -3212,7 +3230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C72" s="33" t="s">
         <v>120</v>
       </c>
@@ -3220,7 +3238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B73" s="50" t="s">
         <v>184</v>
       </c>
@@ -3231,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B74" s="50" t="s">
         <v>187</v>
       </c>
@@ -3239,6 +3257,73 @@
         <v>186</v>
       </c>
       <c r="D74" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B75" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="D75" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D76" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="D77" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="D78" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" s="34">
         <v>1</v>
       </c>
     </row>
@@ -3253,7 +3338,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B67D7FCE-5958-4F9D-8EF5-7923E0C7736A}">
           <x14:formula1>
             <xm:f>Help!$A$2:$A$5</xm:f>

</xml_diff>

<commit_message>
Calendar page: storage summary (in development)
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A1852856-7329-4A9A-913B-3EF9E2B5C72C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8EAC4047-E534-4F7A-A88D-5588A56F8D05}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="198">
   <si>
     <t>№</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>Show dots when many transactions</t>
+  </si>
+  <si>
+    <t>Show day of month for inactive days</t>
+  </si>
+  <si>
+    <t>Make storage as required field</t>
   </si>
 </sst>
 </file>
@@ -2361,11 +2367,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
+      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,11 +2438,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D171)</f>
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-41</v>
+        <v>-44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3325,6 +3331,34 @@
       </c>
       <c r="D79" s="34">
         <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B80" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="D80" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="D81" s="34">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transactions page -> context menu for planned
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A50DF067-22EE-4E72-8BD9-D427707925F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{45C11598-8C98-4EA2-B73B-5289E4A7ACCC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2373,8 +2373,8 @@
   <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2441,11 +2441,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D171)</f>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-48</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2723,14 +2723,15 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="47" t="s">
+      <c r="A25" s="46"/>
+      <c r="B25" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="34">
-        <v>1</v>
+      <c r="D25" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Open storage details by double click
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8794E74B-81F6-49C4-8941-1BB1BFFF0C12}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2D9450D8-0DB9-4488-BA12-AB47996090CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2404,8 +2404,8 @@
   <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2472,11 +2472,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D170)</f>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-58</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2849,14 +2849,15 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="47" t="s">
+      <c r="A33" s="46"/>
+      <c r="B33" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="D33" s="34">
-        <v>1</v>
+      <c r="D33" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3155,14 +3156,15 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="47" t="s">
+      <c r="A61" s="46"/>
+      <c r="B61" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="33" t="s">
+      <c r="C61" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="D61" s="34">
-        <v>1</v>
+      <c r="D61" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Category tree: expand all / collapse all
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2D9450D8-0DB9-4488-BA12-AB47996090CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{94EB31CA-4AB4-4D19-9BD9-423C2331DB2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="214">
   <si>
     <t>№</t>
   </si>
@@ -656,6 +656,21 @@
   </si>
   <si>
     <t>Applying filter on categories takes a lot of time</t>
+  </si>
+  <si>
+    <t>Category view model</t>
+  </si>
+  <si>
+    <t>Remove IsExpandedMainView/IsSelectedMainView</t>
+  </si>
+  <si>
+    <t>Add child</t>
+  </si>
+  <si>
+    <t>Category selector + filter</t>
+  </si>
+  <si>
+    <t>Show inactive</t>
   </si>
 </sst>
 </file>
@@ -2401,11 +2416,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2461,33 +2476,31 @@
       <c r="D2" s="50"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43215</v>
+        <v>43216</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D170)</f>
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-56</v>
+        <v>-59</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
-        <v>123</v>
-      </c>
+      <c r="A3" s="46"/>
       <c r="B3" s="48" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="D3" s="38">
         <v>0</v>
@@ -2499,136 +2512,138 @@
       <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
-        <v>123</v>
-      </c>
+      <c r="A4" s="46"/>
       <c r="B4" s="48" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="D4" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
-        <v>123</v>
-      </c>
+      <c r="A5" s="46"/>
       <c r="B5" s="48" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="D5" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
-        <v>123</v>
-      </c>
+      <c r="A6" s="46"/>
       <c r="B6" s="46" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="D6" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="46"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46" t="s">
+        <v>152</v>
+      </c>
       <c r="C7" s="37" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="D7" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="46"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46" t="s">
+        <v>144</v>
+      </c>
       <c r="C8" s="37" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D8" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="46"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="46" t="s">
+        <v>189</v>
+      </c>
       <c r="C9" s="37" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="D9" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" s="34">
-        <v>2</v>
+      <c r="A10" s="46"/>
+      <c r="B10" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="46"/>
+        <v>123</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>127</v>
+      </c>
       <c r="C11" s="37" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="D11" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="34">
-        <v>1</v>
+      <c r="A12" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="46"/>
+        <v>123</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>127</v>
+      </c>
       <c r="C13" s="37" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="D13" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="46"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="46" t="s">
+        <v>187</v>
+      </c>
       <c r="C14" s="37" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="D14" s="38">
         <v>0</v>
@@ -2636,11 +2651,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="46"/>
+        <v>123</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>128</v>
+      </c>
       <c r="C15" s="37" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="D15" s="38">
         <v>0</v>
@@ -2648,34 +2665,41 @@
     </row>
     <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="46"/>
+        <v>122</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>132</v>
+      </c>
       <c r="C16" s="37" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="D16" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="34">
-        <v>1</v>
+      <c r="A17" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
+      <c r="A18" s="46" t="s">
+        <v>122</v>
+      </c>
       <c r="B18" s="46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>130</v>
+        <v>196</v>
       </c>
       <c r="D18" s="38">
         <v>0</v>
@@ -2684,10 +2708,10 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="46"/>
       <c r="B19" s="46" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="D19" s="38">
         <v>0</v>
@@ -2699,7 +2723,7 @@
         <v>131</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D20" s="38">
         <v>0</v>
@@ -2711,7 +2735,7 @@
         <v>131</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D21" s="38">
         <v>0</v>
@@ -2723,7 +2747,7 @@
         <v>131</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D22" s="38">
         <v>0</v>
@@ -2735,7 +2759,7 @@
         <v>131</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D23" s="38">
         <v>0</v>
@@ -2747,7 +2771,7 @@
         <v>131</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D24" s="38">
         <v>0</v>
@@ -2759,7 +2783,7 @@
         <v>131</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D25" s="38">
         <v>0</v>
@@ -2771,232 +2795,255 @@
         <v>131</v>
       </c>
       <c r="C26" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="46"/>
+      <c r="B27" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="46"/>
+      <c r="B28" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="46" t="s">
+      <c r="D28" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="37" t="s">
+      <c r="B29" s="46"/>
+      <c r="C29" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="46"/>
+      <c r="C30" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="46"/>
+      <c r="C31" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="46"/>
+      <c r="C32" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="46"/>
+      <c r="C35" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="46"/>
+      <c r="C36" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="46"/>
+      <c r="C37" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="46" t="s">
+      <c r="D37" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="37" t="s">
+      <c r="B38" s="46"/>
+      <c r="C38" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="46"/>
-      <c r="B29" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" s="34">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
-      <c r="B31" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="D31" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
-      <c r="B32" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="46"/>
-      <c r="B33" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="C33" s="37" t="s">
+      <c r="D38" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="46"/>
+      <c r="C39" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="46"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="D33" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
-      <c r="B34" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="D34" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="D36" s="34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C37" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="34">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C38" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="34">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="D39" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D40" s="34">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="47" t="s">
-        <v>157</v>
-      </c>
       <c r="C42" s="33" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="D42" s="34">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" s="47" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>133</v>
+        <v>191</v>
       </c>
       <c r="D43" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="47" t="s">
+        <v>123</v>
+      </c>
       <c r="B44" s="47" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>135</v>
+        <v>211</v>
       </c>
       <c r="D44" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="47" t="s">
+        <v>123</v>
+      </c>
       <c r="B45" s="47" t="s">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
       <c r="D45" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="47" t="s">
+        <v>70</v>
+      </c>
       <c r="B46" s="47" t="s">
-        <v>162</v>
+        <v>209</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="D46" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -3004,10 +3051,10 @@
         <v>162</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D47" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -3015,7 +3062,7 @@
         <v>162</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D48" s="34">
         <v>1</v>
@@ -3026,10 +3073,10 @@
         <v>162</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D49" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -3037,29 +3084,35 @@
         <v>162</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D50" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="47" t="s">
+        <v>122</v>
+      </c>
       <c r="B51" s="47" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="D51" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="47" t="s">
+        <v>122</v>
+      </c>
       <c r="B52" s="47" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>168</v>
+        <v>207</v>
       </c>
       <c r="D52" s="34">
         <v>1</v>
@@ -3067,21 +3120,21 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" s="47" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="D53" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B54" s="47" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D54" s="34">
         <v>1</v>
@@ -3089,108 +3142,118 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D57" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="D58" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="C55" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="D55" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B58" s="46"/>
-      <c r="C58" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B59" s="46"/>
-      <c r="C59" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="D59" s="38">
-        <v>0</v>
+      <c r="C59" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="47" t="s">
+      <c r="B60" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="D61" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="46"/>
-      <c r="B61" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="C61" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" s="47" t="s">
         <v>174</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="D62" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="46"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D63" s="38">
-        <v>0</v>
+      <c r="A63" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="D63" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B64" s="47" t="s">
+        <v>182</v>
+      </c>
       <c r="C64" s="33" t="s">
-        <v>82</v>
+        <v>183</v>
       </c>
       <c r="D64" s="34">
         <v>1</v>
@@ -3198,54 +3261,60 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B65" s="47" t="s">
-        <v>189</v>
+        <v>131</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="D65" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="47" t="s">
+        <v>117</v>
+      </c>
       <c r="B66" s="47" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="D66" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="47" t="s">
+        <v>122</v>
+      </c>
       <c r="B67" s="47" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="D67" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B68" s="47" t="s">
-        <v>178</v>
+      <c r="A68" s="47" t="s">
+        <v>70</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>177</v>
+        <v>75</v>
       </c>
       <c r="D68" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B69" s="47" t="s">
-        <v>178</v>
+      <c r="A69" s="47" t="s">
+        <v>70</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>179</v>
+        <v>84</v>
       </c>
       <c r="D69" s="34">
         <v>1</v>
@@ -3253,148 +3322,128 @@
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="C70" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="D70" s="34">
+      <c r="C71" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D71" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D72" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C73" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D73" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C74" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="D74" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="D75" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B76" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B71" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="C71" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="D71" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C72" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D72" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="46"/>
-      <c r="B73" s="46" t="s">
-        <v>184</v>
-      </c>
-      <c r="C73" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="D73" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="46"/>
-      <c r="B74" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="C74" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="D74" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="C75" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="D75" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B76" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C76" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="D76" s="38">
-        <v>0</v>
-      </c>
-    </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B77" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C77" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="D77" s="38">
-        <v>0</v>
+      <c r="B77" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="34">
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="47" t="s">
-        <v>122</v>
-      </c>
       <c r="B78" s="47" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="D78" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B79" s="47" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="D79" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B80" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="C80" s="37" t="s">
-        <v>196</v>
-      </c>
-      <c r="D80" s="38">
-        <v>0</v>
+      <c r="B80" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="34">
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B81" s="47" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="D81" s="34">
         <v>2</v>
@@ -3402,119 +3451,135 @@
     </row>
     <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B82" s="47" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="C82" s="33" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="D82" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="47" t="s">
+        <v>70</v>
+      </c>
       <c r="C83" s="33" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="D83" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="B84" s="47" t="s">
-        <v>200</v>
-      </c>
       <c r="C84" s="33" t="s">
-        <v>201</v>
+        <v>73</v>
       </c>
       <c r="D84" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="47" t="s">
-        <v>70</v>
-      </c>
       <c r="B85" s="47" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="C85" s="33" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="D85" s="34">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="47" t="s">
-        <v>122</v>
+      <c r="B86" s="47" t="s">
+        <v>162</v>
       </c>
       <c r="C86" s="33" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="D86" s="34">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="47" t="s">
-        <v>123</v>
-      </c>
       <c r="B87" s="47" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C87" s="33" t="s">
-        <v>205</v>
+        <v>133</v>
       </c>
       <c r="D87" s="34">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="47" t="s">
-        <v>123</v>
-      </c>
       <c r="B88" s="47" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C88" s="33" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="D88" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="47" t="s">
-        <v>122</v>
-      </c>
       <c r="B89" s="47" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="C89" s="33" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="D89" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="47" t="s">
-        <v>117</v>
-      </c>
       <c r="B90" s="47" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C90" s="33" t="s">
-        <v>208</v>
+        <v>143</v>
       </c>
       <c r="D90" s="34">
-        <v>1</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B91" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C91" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="D91" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C92" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C93" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D93" s="34">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A4:D93">
+    <sortCondition ref="D3:D93"/>
+    <sortCondition ref="B3:B93"/>
+  </sortState>
   <mergeCells count="4">
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>

</xml_diff>

<commit_message>
Data filter -> category seletor context menu
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{94EB31CA-4AB4-4D19-9BD9-423C2331DB2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C0AFD3CF-5FD1-4F0A-A868-B7A05770C9CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="215">
   <si>
     <t>№</t>
   </si>
@@ -671,6 +671,9 @@
   </si>
   <si>
     <t>Show inactive</t>
+  </si>
+  <si>
+    <t>Save IsCategoryBranchSelection to database</t>
   </si>
 </sst>
 </file>
@@ -2416,11 +2419,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
+      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2487,11 +2490,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D170)</f>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-59</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3414,17 +3417,17 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="47" t="s">
+      <c r="A79" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B79" s="47" t="s">
+      <c r="B79" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="33" t="s">
+      <c r="C79" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="D79" s="34">
-        <v>2</v>
+      <c r="D79" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3573,6 +3576,17 @@
       </c>
       <c r="D93" s="34">
         <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B94" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="D94" s="34">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Categories page -> Add child category
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C0AFD3CF-5FD1-4F0A-A868-B7A05770C9CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DE9BBD49-7AC7-480F-B25C-74282CD7F3BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="217">
   <si>
     <t>№</t>
   </si>
@@ -674,6 +674,12 @@
   </si>
   <si>
     <t>Save IsCategoryBranchSelection to database</t>
+  </si>
+  <si>
+    <t>Add record/money transfer to separate buttons</t>
+  </si>
+  <si>
+    <t>Create mini menu with buttons from context menu</t>
   </si>
 </sst>
 </file>
@@ -2419,11 +2425,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2490,11 +2496,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D170)</f>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-58</v>
+        <v>-59</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3008,17 +3014,17 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="D44" s="34">
-        <v>1</v>
+      <c r="D44" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -3579,6 +3585,9 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="47" t="s">
+        <v>122</v>
+      </c>
       <c r="B94" s="47" t="s">
         <v>180</v>
       </c>
@@ -3586,6 +3595,34 @@
         <v>214</v>
       </c>
       <c r="D94" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B95" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="D95" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B96" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C96" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="D96" s="34">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Categories page -> toolbar expand/collapse all buttons
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DE9BBD49-7AC7-480F-B25C-74282CD7F3BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0C2B3CD9-DBD4-4205-A481-6B8F57E119BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="216">
   <si>
     <t>№</t>
   </si>
@@ -670,16 +670,13 @@
     <t>Category selector + filter</t>
   </si>
   <si>
-    <t>Show inactive</t>
-  </si>
-  <si>
     <t>Save IsCategoryBranchSelection to database</t>
   </si>
   <si>
     <t>Add record/money transfer to separate buttons</t>
   </si>
   <si>
-    <t>Create mini menu with buttons from context menu</t>
+    <t>Show inactive + tool bar for expand/collapse all</t>
   </si>
 </sst>
 </file>
@@ -2425,11 +2422,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2496,11 +2493,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D170)</f>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-59</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3035,7 +3032,7 @@
         <v>212</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D45" s="34">
         <v>1</v>
@@ -3592,7 +3589,7 @@
         <v>180</v>
       </c>
       <c r="C94" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D94" s="34">
         <v>1</v>
@@ -3606,23 +3603,9 @@
         <v>131</v>
       </c>
       <c r="C95" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D95" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="B96" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="C96" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="D96" s="34">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Planning page -> update context menu
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0C2B3CD9-DBD4-4205-A481-6B8F57E119BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9B8B8EE7-486D-43BC-B898-5FC50DA56B1E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2425,8 +2425,8 @@
   <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
+      <pane ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2493,11 +2493,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D170)</f>
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-58</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3136,25 +3136,27 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="47" t="s">
+      <c r="A54" s="46"/>
+      <c r="B54" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C54" s="33" t="s">
+      <c r="C54" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="D54" s="34">
-        <v>1</v>
+      <c r="D54" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="47" t="s">
+      <c r="A55" s="46"/>
+      <c r="B55" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C55" s="33" t="s">
+      <c r="C55" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="D55" s="34">
-        <v>1</v>
+      <c r="D55" s="38">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Storages page -> money transfers filter
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{12B5FE5E-1953-4FD1-AE9B-24813631AB6E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7938CC3D-5775-45B2-8FE9-06213335F1D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="224">
   <si>
     <t>№</t>
   </si>
@@ -695,6 +695,12 @@
   </si>
   <si>
     <t>Add possibility to add new category</t>
+  </si>
+  <si>
+    <t>Refactor commands</t>
+  </si>
+  <si>
+    <t>Save columns order and size</t>
   </si>
 </sst>
 </file>
@@ -2440,11 +2446,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M99"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
+      <pane ySplit="2" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2511,11 +2517,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D170)</f>
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-59</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3640,7 +3646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B97" s="44" t="s">
         <v>139</v>
       </c>
@@ -3651,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B98" s="44" t="s">
         <v>218</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B99" s="44" t="s">
         <v>220</v>
       </c>
@@ -3670,6 +3676,31 @@
         <v>221</v>
       </c>
       <c r="D99" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C100" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="D100" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B101" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C101" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="D101" s="33">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add cheque -> Show total amount
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7938CC3D-5775-45B2-8FE9-06213335F1D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8828EE65-E398-4328-8412-0D07EC7C0FCC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Help" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Estimate!$A$1:$A$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Estimate!$A$1:$A$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plans!$A$1:$E$52</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="226">
   <si>
     <t>№</t>
   </si>
@@ -577,12 +577,6 @@
     <t>Category tree context menu (expand all, collapse all, select all, upselect all, select branch, unselect branch)</t>
   </si>
   <si>
-    <t>Transactions Page</t>
-  </si>
-  <si>
-    <t>Show/hide planned transactions</t>
-  </si>
-  <si>
     <t>Debts list</t>
   </si>
   <si>
@@ -604,9 +598,6 @@
     <t>Ограничения на строки</t>
   </si>
   <si>
-    <t>Cell height in settings</t>
-  </si>
-  <si>
     <t>When change income/expence resultat amount isn't changed</t>
   </si>
   <si>
@@ -701,6 +692,21 @@
   </si>
   <si>
     <t>Save columns order and size</t>
+  </si>
+  <si>
+    <t>Cell height in settings / max transactions count</t>
+  </si>
+  <si>
+    <t>Refactor filters</t>
+  </si>
+  <si>
+    <t>Code cleanup</t>
+  </si>
+  <si>
+    <t>DublicateCommand</t>
+  </si>
+  <si>
+    <t>Add defaults provider</t>
   </si>
 </sst>
 </file>
@@ -2446,11 +2452,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2506,31 +2512,33 @@
       <c r="D2" s="47"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43217</v>
+        <v>43218</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J2" s="25">
-        <f>SUM(D3:D170)</f>
-        <v>126</v>
+        <f>SUM(D3:D169)</f>
+        <v>124</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-61</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="43"/>
+      <c r="A3" s="43" t="s">
+        <v>122</v>
+      </c>
       <c r="B3" s="45" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>151</v>
+        <v>204</v>
       </c>
       <c r="D3" s="36">
         <v>0</v>
@@ -2542,72 +2550,80 @@
       <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="43"/>
+      <c r="A4" s="43" t="s">
+        <v>122</v>
+      </c>
       <c r="B4" s="45" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="D4" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="43"/>
+      <c r="A5" s="43" t="s">
+        <v>122</v>
+      </c>
       <c r="B5" s="45" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="D5" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
+      <c r="A6" s="43" t="s">
+        <v>122</v>
+      </c>
       <c r="B6" s="43" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="D6" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
+      <c r="A7" s="43" t="s">
+        <v>122</v>
+      </c>
       <c r="B7" s="43" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="D7" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43" t="s">
-        <v>144</v>
-      </c>
+      <c r="A8" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="43"/>
       <c r="C8" s="50" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="D8" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43" t="s">
-        <v>189</v>
-      </c>
+      <c r="A9" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="43"/>
       <c r="C9" s="50" t="s">
-        <v>188</v>
+        <v>97</v>
       </c>
       <c r="D9" s="36">
         <v>0</v>
@@ -2615,13 +2631,11 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>189</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B10" s="43"/>
       <c r="C10" s="50" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D10" s="36">
         <v>0</v>
@@ -2629,13 +2643,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="43" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D11" s="36">
         <v>0</v>
@@ -2656,12 +2670,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
+      <c r="A13" s="43" t="s">
+        <v>123</v>
+      </c>
       <c r="B13" s="43" t="s">
-        <v>184</v>
+        <v>127</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>185</v>
+        <v>92</v>
       </c>
       <c r="D13" s="36">
         <v>0</v>
@@ -2675,7 +2691,7 @@
         <v>127</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D14" s="36">
         <v>0</v>
@@ -2689,7 +2705,7 @@
         <v>127</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D15" s="36">
         <v>0</v>
@@ -2700,46 +2716,48 @@
         <v>123</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="D16" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="43"/>
+      <c r="A17" s="43" t="s">
+        <v>123</v>
+      </c>
       <c r="B17" s="43" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="D17" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43" t="s">
-        <v>178</v>
-      </c>
+      <c r="A18" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="43"/>
       <c r="C18" s="50" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="D18" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43" t="s">
-        <v>187</v>
-      </c>
+      <c r="A19" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="43"/>
       <c r="C19" s="50" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="D19" s="36">
         <v>0</v>
@@ -2747,13 +2765,11 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>128</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B20" s="43"/>
       <c r="C20" s="50" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="D20" s="36">
         <v>0</v>
@@ -2761,13 +2777,11 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>132</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B21" s="43"/>
       <c r="C21" s="50" t="s">
-        <v>192</v>
+        <v>148</v>
       </c>
       <c r="D21" s="36">
         <v>0</v>
@@ -2775,13 +2789,11 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>132</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B22" s="43"/>
       <c r="C22" s="50" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="D22" s="36">
         <v>0</v>
@@ -2789,61 +2801,59 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="43" t="s">
-        <v>132</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B23" s="43"/>
       <c r="C23" s="50" t="s">
-        <v>196</v>
+        <v>89</v>
       </c>
       <c r="D23" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43" t="s">
-        <v>174</v>
-      </c>
+      <c r="A24" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="43"/>
       <c r="C24" s="50" t="s">
-        <v>173</v>
+        <v>90</v>
       </c>
       <c r="D24" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43" t="s">
-        <v>131</v>
-      </c>
+      <c r="A25" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="43"/>
       <c r="C25" s="50" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D25" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43" t="s">
-        <v>131</v>
-      </c>
+      <c r="A26" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="43"/>
       <c r="C26" s="50" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D26" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43" t="s">
-        <v>131</v>
-      </c>
+      <c r="A27" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="43"/>
       <c r="C27" s="50" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D27" s="36">
         <v>0</v>
@@ -2852,10 +2862,10 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
       <c r="B28" s="43" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="D28" s="36">
         <v>0</v>
@@ -2864,7 +2874,7 @@
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="43"/>
       <c r="B29" s="43" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C29" s="50" t="s">
         <v>135</v>
@@ -2876,10 +2886,10 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="43"/>
       <c r="B30" s="43" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="D30" s="36">
         <v>0</v>
@@ -2888,10 +2898,10 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="43"/>
       <c r="B31" s="43" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="D31" s="36">
         <v>0</v>
@@ -2900,10 +2910,10 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="43"/>
       <c r="B32" s="43" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="D32" s="36">
         <v>0</v>
@@ -2912,168 +2922,166 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="43"/>
       <c r="B33" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="D33" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="43"/>
+      <c r="B34" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="43"/>
+      <c r="B35" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="43"/>
+      <c r="B37" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="C37" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="43"/>
+      <c r="B38" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="D38" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="43"/>
+      <c r="B39" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="43"/>
+      <c r="B40" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="43"/>
+      <c r="B41" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="43"/>
+      <c r="B42" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="50" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>200</v>
-      </c>
-      <c r="C34" s="50" t="s">
-        <v>201</v>
-      </c>
-      <c r="D34" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="D35" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="50" t="s">
-        <v>145</v>
-      </c>
-      <c r="D36" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="50" t="s">
-        <v>146</v>
-      </c>
-      <c r="D37" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="D38" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="D39" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="43"/>
-      <c r="C40" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="43"/>
-      <c r="C41" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="43"/>
       <c r="C42" s="50" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D42" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="43"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43" t="s">
+        <v>131</v>
+      </c>
       <c r="C43" s="50" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D43" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="43"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43" t="s">
+        <v>131</v>
+      </c>
       <c r="C44" s="50" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D44" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B45" s="43"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43" t="s">
+        <v>131</v>
+      </c>
       <c r="C45" s="50" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="D45" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B46" s="43"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43" t="s">
+        <v>131</v>
+      </c>
       <c r="C46" s="50" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="D46" s="36">
         <v>0</v>
@@ -3081,106 +3089,113 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="43"/>
-      <c r="B47" s="43"/>
+      <c r="B47" s="43" t="s">
+        <v>131</v>
+      </c>
       <c r="C47" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="43"/>
+      <c r="B48" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="43"/>
+      <c r="B49" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="43"/>
+      <c r="B50" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="43"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="44" t="s">
+      <c r="D51" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B52" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="D52" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="C48" s="51" t="s">
-        <v>195</v>
-      </c>
-      <c r="D48" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="44" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="51" t="s">
+      <c r="C53" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="D53" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="D49" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="B50" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="C50" s="51" t="s">
-        <v>215</v>
-      </c>
-      <c r="D50" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="C51" s="51" t="s">
+      <c r="D54" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="51" t="s">
         <v>210</v>
-      </c>
-      <c r="D51" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B52" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="C52" s="51" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B53" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="C53" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="D53" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>167</v>
-      </c>
-      <c r="D54" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="51" t="s">
-        <v>168</v>
       </c>
       <c r="D55" s="33">
         <v>1</v>
@@ -3191,10 +3206,10 @@
         <v>122</v>
       </c>
       <c r="B56" s="44" t="s">
-        <v>180</v>
+        <v>127</v>
       </c>
       <c r="C56" s="51" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D56" s="33">
         <v>1</v>
@@ -3204,55 +3219,64 @@
       <c r="A57" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="B57" s="44" t="s">
-        <v>180</v>
-      </c>
       <c r="C57" s="51" t="s">
-        <v>213</v>
+        <v>72</v>
       </c>
       <c r="D57" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B58" s="44" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C58" s="51" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="D58" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B59" s="44" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="C59" s="51" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D59" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B60" s="44" t="s">
-        <v>157</v>
+        <v>209</v>
       </c>
       <c r="C60" s="51" t="s">
-        <v>159</v>
+        <v>212</v>
       </c>
       <c r="D60" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B61" s="44" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C61" s="51" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="D61" s="33">
         <v>1</v>
@@ -3260,46 +3284,55 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="44" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="B62" s="44" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="C62" s="51" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="D62" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B63" s="44" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C63" s="51" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D63" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B64" s="44" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C64" s="51" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D64" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B65" s="44" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="D65" s="33">
         <v>1</v>
@@ -3310,10 +3343,10 @@
         <v>123</v>
       </c>
       <c r="B66" s="44" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C66" s="51" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D66" s="33">
         <v>1</v>
@@ -3324,32 +3357,38 @@
         <v>123</v>
       </c>
       <c r="B67" s="44" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C67" s="51" t="s">
-        <v>206</v>
+        <v>159</v>
       </c>
       <c r="D67" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B68" s="44" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="C68" s="51" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="D68" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B69" s="44" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="C69" s="51" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="D69" s="33">
         <v>1</v>
@@ -3357,13 +3396,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="44" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B70" s="44" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="C70" s="51" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="D70" s="33">
         <v>1</v>
@@ -3374,10 +3413,10 @@
         <v>123</v>
       </c>
       <c r="B71" s="44" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="C71" s="51" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="D71" s="33">
         <v>1</v>
@@ -3385,10 +3424,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="44" t="s">
-        <v>70</v>
+        <v>123</v>
+      </c>
+      <c r="B72" s="44" t="s">
+        <v>174</v>
       </c>
       <c r="C72" s="51" t="s">
-        <v>75</v>
+        <v>203</v>
       </c>
       <c r="D72" s="33">
         <v>1</v>
@@ -3396,10 +3438,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="44" t="s">
-        <v>70</v>
+        <v>123</v>
+      </c>
+      <c r="B73" s="44" t="s">
+        <v>131</v>
       </c>
       <c r="C73" s="51" t="s">
-        <v>84</v>
+        <v>211</v>
       </c>
       <c r="D73" s="33">
         <v>1</v>
@@ -3407,10 +3452,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="44" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C74" s="51" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D74" s="33">
         <v>1</v>
@@ -3421,7 +3466,7 @@
         <v>123</v>
       </c>
       <c r="C75" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D75" s="33">
         <v>1</v>
@@ -3432,111 +3477,126 @@
         <v>123</v>
       </c>
       <c r="C76" s="51" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="D76" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="C77" s="51" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="D77" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78" s="44" t="s">
+        <v>131</v>
+      </c>
       <c r="C78" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="D78" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="C79" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="D79" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="D78" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C79" s="51" t="s">
-        <v>204</v>
-      </c>
-      <c r="D79" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B80" s="44" t="s">
-        <v>152</v>
-      </c>
       <c r="C80" s="51" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D80" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="44" t="s">
-        <v>162</v>
+      <c r="A81" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="C81" s="51" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
       <c r="D81" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B82" s="44" t="s">
-        <v>162</v>
+      <c r="A82" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="C82" s="51" t="s">
-        <v>165</v>
+        <v>84</v>
       </c>
       <c r="D82" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B83" s="44" t="s">
-        <v>157</v>
+      <c r="A83" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="C83" s="51" t="s">
-        <v>151</v>
+        <v>219</v>
       </c>
       <c r="D83" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B84" s="44" t="s">
-        <v>157</v>
+      <c r="A84" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="C84" s="51" t="s">
-        <v>161</v>
+        <v>222</v>
       </c>
       <c r="D84" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B85" s="44" t="s">
-        <v>171</v>
+      <c r="A85" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="C85" s="51" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="D85" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="44" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="C86" s="51" t="s">
-        <v>147</v>
+        <v>73</v>
       </c>
       <c r="D86" s="33">
         <v>2</v>
@@ -3544,170 +3604,252 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="44" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="B87" s="44" t="s">
+        <v>162</v>
       </c>
       <c r="C87" s="51" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="D87" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B88" s="44" t="s">
         <v>162</v>
       </c>
       <c r="C88" s="51" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D88" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B89" s="44" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C89" s="51" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D89" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="B90" s="44" t="s">
         <v>157</v>
       </c>
       <c r="C90" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B91" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D91" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B92" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="C92" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="D92" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C93" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B94" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C94" s="51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D94" s="33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B95" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C95" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="D95" s="33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B96" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C96" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="D90" s="33">
+      <c r="D96" s="33">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B91" s="44" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B97" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="C91" s="51" t="s">
+      <c r="C97" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="D91" s="33">
+      <c r="D97" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="44" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B98" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="C92" s="51" t="s">
+      <c r="C98" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="D92" s="33">
+      <c r="D98" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B93" s="44" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B99" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="C93" s="51" t="s">
+      <c r="C99" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="D93" s="33">
+      <c r="D99" s="33">
         <v>7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="C94" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="D94" s="33">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C95" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="D95" s="33">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C96" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="D96" s="33">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B97" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="C97" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="D97" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B98" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="C98" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="D98" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="C99" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="D99" s="33">
-        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="44" t="s">
-        <v>70</v>
+        <v>123</v>
+      </c>
+      <c r="B100" s="44" t="s">
+        <v>157</v>
       </c>
       <c r="C100" s="51" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="D100" s="33">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="B101" s="44" t="s">
-        <v>110</v>
-      </c>
       <c r="C101" s="51" t="s">
-        <v>223</v>
+        <v>15</v>
       </c>
       <c r="D101" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C102" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B103" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C103" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="C104" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="D104" s="33">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:D96">
-    <sortCondition ref="D3:D96"/>
-    <sortCondition ref="B3:B96"/>
+  <sortState ref="A4:D102">
+    <sortCondition ref="D3:D102"/>
+    <sortCondition ref="A3:A102"/>
+    <sortCondition ref="B3:B102"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="C1:C2"/>

</xml_diff>

<commit_message>
Minor fixea and closed limits cleanup
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5BE7C28B-2350-4C5D-9A2F-35F5C5311194}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CDECF3EA-E4C9-4511-B831-120307DEF956}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="243">
   <si>
     <t>№</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Storage page -&gt; summary for every group</t>
   </si>
   <si>
-    <t>Storage group -&gt; серый цвет</t>
-  </si>
-  <si>
     <t>Header окна + название выбранной страницы</t>
   </si>
   <si>
@@ -730,12 +727,6 @@
     <t>Insert calculator everywhere for enter amount</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove ServiceManager. Use </t>
-  </si>
-  <si>
-    <t>Main calendar. Use ListView instead of Grid</t>
-  </si>
-  <si>
     <t>Action type is not refreshed after change</t>
   </si>
   <si>
@@ -754,9 +745,6 @@
     <t xml:space="preserve">Advice generator </t>
   </si>
   <si>
-    <t>Add possibility to update current</t>
-  </si>
-  <si>
     <t>Currency exchange rate</t>
   </si>
   <si>
@@ -764,6 +752,12 @@
   </si>
   <si>
     <t>When select debt currency is not recognized</t>
+  </si>
+  <si>
+    <t>Add possibility to update current in record details</t>
+  </si>
+  <si>
+    <t>Remove ServiceManager. Use Autofac</t>
   </si>
 </sst>
 </file>
@@ -2509,11 +2503,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
+      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,10 +2529,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="49" t="s">
         <v>2</v>
@@ -2559,7 +2553,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2569,33 +2563,33 @@
       <c r="D2" s="50"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43220</v>
+        <v>43221</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J2" s="25">
-        <f>SUM(D3:D168)</f>
-        <v>92</v>
+        <f>SUM(D3:D167)</f>
+        <v>107</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-30</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" s="36">
         <v>0</v>
@@ -2608,13 +2602,13 @@
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D4" s="36">
         <v>0</v>
@@ -2622,13 +2616,13 @@
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D5" s="36">
         <v>0</v>
@@ -2636,13 +2630,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D6" s="36">
         <v>0</v>
@@ -2650,13 +2644,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" s="36">
         <v>0</v>
@@ -2664,13 +2658,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="47" t="s">
         <v>196</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>197</v>
       </c>
       <c r="D8" s="36">
         <v>0</v>
@@ -2678,7 +2672,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="47" t="s">
@@ -2690,11 +2684,11 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="36">
         <v>0</v>
@@ -2702,11 +2696,11 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" s="43"/>
       <c r="C11" s="47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D11" s="36">
         <v>0</v>
@@ -2714,13 +2708,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12" s="36">
         <v>0</v>
@@ -2728,13 +2722,13 @@
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="47" t="s">
         <v>179</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>180</v>
       </c>
       <c r="D13" s="36">
         <v>0</v>
@@ -2742,13 +2736,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" s="36">
         <v>0</v>
@@ -2756,13 +2750,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="36">
         <v>0</v>
@@ -2770,13 +2764,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="36">
         <v>0</v>
@@ -2784,13 +2778,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="47" t="s">
         <v>127</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>128</v>
       </c>
       <c r="D17" s="36">
         <v>0</v>
@@ -2798,13 +2792,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D18" s="36">
         <v>0</v>
@@ -2816,7 +2810,7 @@
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" s="36">
         <v>0</v>
@@ -2828,7 +2822,7 @@
       </c>
       <c r="B20" s="43"/>
       <c r="C20" s="47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="36">
         <v>0</v>
@@ -2840,7 +2834,7 @@
       </c>
       <c r="B21" s="43"/>
       <c r="C21" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D21" s="36">
         <v>0</v>
@@ -2852,7 +2846,7 @@
       </c>
       <c r="B22" s="43"/>
       <c r="C22" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D22" s="36">
         <v>0</v>
@@ -2864,7 +2858,7 @@
       </c>
       <c r="B23" s="43"/>
       <c r="C23" s="47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D23" s="36">
         <v>0</v>
@@ -2876,7 +2870,7 @@
       </c>
       <c r="B24" s="43"/>
       <c r="C24" s="47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D24" s="36">
         <v>0</v>
@@ -2888,7 +2882,7 @@
       </c>
       <c r="B25" s="43"/>
       <c r="C25" s="47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="36">
         <v>0</v>
@@ -2900,7 +2894,7 @@
       </c>
       <c r="B26" s="43"/>
       <c r="C26" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D26" s="36">
         <v>0</v>
@@ -2912,7 +2906,7 @@
       </c>
       <c r="B27" s="43"/>
       <c r="C27" s="47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D27" s="36">
         <v>0</v>
@@ -2924,7 +2918,7 @@
       </c>
       <c r="B28" s="43"/>
       <c r="C28" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D28" s="36">
         <v>0</v>
@@ -2933,10 +2927,10 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="43"/>
       <c r="B29" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="36">
         <v>0</v>
@@ -2945,10 +2939,10 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="43"/>
       <c r="B30" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" s="36">
         <v>0</v>
@@ -2957,10 +2951,10 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="43"/>
       <c r="B31" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="47" t="s">
         <v>151</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>152</v>
       </c>
       <c r="D31" s="36">
         <v>0</v>
@@ -2969,10 +2963,10 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="43"/>
       <c r="B32" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D32" s="36">
         <v>0</v>
@@ -2981,10 +2975,10 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="43"/>
       <c r="B33" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D33" s="36">
         <v>0</v>
@@ -2993,10 +2987,10 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="43"/>
       <c r="B34" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C34" s="47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D34" s="36">
         <v>0</v>
@@ -3005,10 +2999,10 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" s="36">
         <v>0</v>
@@ -3017,10 +3011,10 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="43"/>
       <c r="B36" s="43" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D36" s="36">
         <v>0</v>
@@ -3029,10 +3023,10 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="43"/>
       <c r="B37" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="47" t="s">
         <v>214</v>
-      </c>
-      <c r="C37" s="47" t="s">
-        <v>215</v>
       </c>
       <c r="D37" s="36">
         <v>0</v>
@@ -3041,10 +3035,10 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="43"/>
       <c r="B38" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="47" t="s">
         <v>181</v>
-      </c>
-      <c r="C38" s="47" t="s">
-        <v>182</v>
       </c>
       <c r="D38" s="36">
         <v>0</v>
@@ -3053,10 +3047,10 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="43"/>
       <c r="B39" s="43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D39" s="36">
         <v>0</v>
@@ -3065,10 +3059,10 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="43"/>
       <c r="B40" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="47" t="s">
         <v>177</v>
-      </c>
-      <c r="C40" s="47" t="s">
-        <v>178</v>
       </c>
       <c r="D40" s="36">
         <v>0</v>
@@ -3077,10 +3071,10 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="43"/>
       <c r="B41" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D41" s="36">
         <v>0</v>
@@ -3089,10 +3083,10 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="43"/>
       <c r="B42" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C42" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D42" s="36">
         <v>0</v>
@@ -3101,10 +3095,10 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="43"/>
       <c r="B43" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C43" s="47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" s="36">
         <v>0</v>
@@ -3113,10 +3107,10 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="43"/>
       <c r="B44" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="47" t="s">
         <v>130</v>
-      </c>
-      <c r="C44" s="47" t="s">
-        <v>131</v>
       </c>
       <c r="D44" s="36">
         <v>0</v>
@@ -3125,10 +3119,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="43"/>
       <c r="B45" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D45" s="36">
         <v>0</v>
@@ -3137,10 +3131,10 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="43"/>
       <c r="B46" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D46" s="36">
         <v>0</v>
@@ -3149,10 +3143,10 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="43"/>
       <c r="B47" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D47" s="36">
         <v>0</v>
@@ -3161,10 +3155,10 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="43"/>
       <c r="B48" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D48" s="36">
         <v>0</v>
@@ -3173,10 +3167,10 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="43"/>
       <c r="B49" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C49" s="47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D49" s="36">
         <v>0</v>
@@ -3185,10 +3179,10 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="43"/>
       <c r="B50" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D50" s="36">
         <v>0</v>
@@ -3197,10 +3191,10 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="43"/>
       <c r="B51" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C51" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D51" s="36">
         <v>0</v>
@@ -3210,7 +3204,7 @@
       <c r="A52" s="43"/>
       <c r="B52" s="43"/>
       <c r="C52" s="47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D52" s="36">
         <v>0</v>
@@ -3218,13 +3212,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C53" s="47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D53" s="36">
         <v>0</v>
@@ -3232,13 +3226,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B54" s="43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C54" s="47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D54" s="36">
         <v>0</v>
@@ -3246,13 +3240,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D55" s="36">
         <v>0</v>
@@ -3260,7 +3254,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B56" s="43"/>
       <c r="C56" s="47" t="s">
@@ -3272,13 +3266,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B57" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C57" s="47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D57" s="36">
         <v>0</v>
@@ -3286,13 +3280,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C58" s="47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D58" s="36">
         <v>0</v>
@@ -3300,13 +3294,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C59" s="47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D59" s="36">
         <v>0</v>
@@ -3314,13 +3308,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="C60" s="47" t="s">
         <v>216</v>
-      </c>
-      <c r="C60" s="47" t="s">
-        <v>217</v>
       </c>
       <c r="D60" s="36">
         <v>0</v>
@@ -3328,13 +3322,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C61" s="47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D61" s="36">
         <v>0</v>
@@ -3342,13 +3336,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B62" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D62" s="33">
         <v>1</v>
@@ -3356,13 +3350,13 @@
     </row>
     <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B63" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D63" s="33">
         <v>1</v>
@@ -3370,13 +3364,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B64" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D64" s="33">
         <v>1</v>
@@ -3384,13 +3378,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B65" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D65" s="33">
         <v>1</v>
@@ -3398,13 +3392,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B66" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D66" s="33">
         <v>1</v>
@@ -3412,13 +3406,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C67" s="47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D67" s="36">
         <v>0</v>
@@ -3426,13 +3420,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B68" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C68" s="48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D68" s="33">
         <v>1</v>
@@ -3440,13 +3434,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B69" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D69" s="33">
         <v>1</v>
@@ -3454,13 +3448,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B70" s="44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D70" s="33">
         <v>1</v>
@@ -3468,13 +3462,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C71" s="48" t="s">
         <v>173</v>
-      </c>
-      <c r="C71" s="48" t="s">
-        <v>174</v>
       </c>
       <c r="D71" s="33">
         <v>1</v>
@@ -3482,13 +3476,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B72" s="44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C72" s="48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D72" s="33">
         <v>1</v>
@@ -3496,38 +3490,38 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B73" s="44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C73" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D73" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="B74" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D74" s="33">
-        <v>1</v>
+      <c r="A74" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="D74" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C75" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D75" s="33">
         <v>1</v>
@@ -3535,10 +3529,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C76" s="48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D76" s="33">
         <v>1</v>
@@ -3546,10 +3540,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C77" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D77" s="33">
         <v>1</v>
@@ -3557,10 +3551,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C78" s="48" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D78" s="33">
         <v>1</v>
@@ -3568,13 +3562,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C79" s="47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D79" s="36">
         <v>0</v>
@@ -3585,10 +3579,10 @@
         <v>70</v>
       </c>
       <c r="B80" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="C80" s="48" t="s">
         <v>205</v>
-      </c>
-      <c r="C80" s="48" t="s">
-        <v>206</v>
       </c>
       <c r="D80" s="33">
         <v>1</v>
@@ -3599,10 +3593,10 @@
         <v>70</v>
       </c>
       <c r="B81" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="C81" s="48" t="s">
         <v>198</v>
-      </c>
-      <c r="C81" s="48" t="s">
-        <v>199</v>
       </c>
       <c r="D81" s="33">
         <v>1</v>
@@ -3613,10 +3607,10 @@
         <v>70</v>
       </c>
       <c r="B82" s="44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C82" s="48" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D82" s="33">
         <v>1</v>
@@ -3638,7 +3632,7 @@
         <v>70</v>
       </c>
       <c r="C84" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D84" s="33">
         <v>1</v>
@@ -3649,7 +3643,7 @@
         <v>70</v>
       </c>
       <c r="C85" s="48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D85" s="33">
         <v>1</v>
@@ -3660,7 +3654,7 @@
         <v>70</v>
       </c>
       <c r="C86" s="48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D86" s="33">
         <v>1</v>
@@ -3671,7 +3665,7 @@
         <v>70</v>
       </c>
       <c r="C87" s="48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D87" s="33">
         <v>1</v>
@@ -3679,10 +3673,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C88" s="48" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D88" s="33">
         <v>2</v>
@@ -3690,13 +3684,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B89" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C89" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D89" s="33">
         <v>2</v>
@@ -3704,13 +3698,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B90" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C90" s="48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D90" s="33">
         <v>2</v>
@@ -3718,13 +3712,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B91" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C91" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D91" s="33">
         <v>2</v>
@@ -3732,13 +3726,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B92" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C92" s="48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D92" s="33">
         <v>2</v>
@@ -3746,13 +3740,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B93" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="C93" s="48" t="s">
         <v>170</v>
-      </c>
-      <c r="C93" s="48" t="s">
-        <v>171</v>
       </c>
       <c r="D93" s="33">
         <v>2</v>
@@ -3760,13 +3754,13 @@
     </row>
     <row r="94" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B94" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C94" s="48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D94" s="33">
         <v>2</v>
@@ -3777,7 +3771,7 @@
         <v>70</v>
       </c>
       <c r="C95" s="48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D95" s="33">
         <v>2</v>
@@ -3785,13 +3779,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B96" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C96" s="48" t="s">
         <v>161</v>
-      </c>
-      <c r="C96" s="48" t="s">
-        <v>162</v>
       </c>
       <c r="D96" s="33">
         <v>3</v>
@@ -3799,13 +3793,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B97" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C97" s="48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D97" s="33">
         <v>3</v>
@@ -3813,13 +3807,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B98" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C98" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D98" s="33">
         <v>3</v>
@@ -3827,13 +3821,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B99" s="44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D99" s="33">
         <v>4</v>
@@ -3841,13 +3835,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B100" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D100" s="33">
         <v>4</v>
@@ -3855,13 +3849,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B101" s="44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D101" s="33">
         <v>7</v>
@@ -3869,13 +3863,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B102" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="C102" s="48" t="s">
         <v>156</v>
-      </c>
-      <c r="C102" s="48" t="s">
-        <v>157</v>
       </c>
       <c r="D102" s="33">
         <v>7</v>
@@ -3883,7 +3877,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C103" s="48" t="s">
         <v>15</v>
@@ -3894,10 +3888,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D104" s="33">
         <v>10</v>
@@ -3905,13 +3899,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B105" s="44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D105" s="33">
         <v>1</v>
@@ -3919,10 +3913,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="D106" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -3931,7 +3928,7 @@
       </c>
       <c r="B107" s="43"/>
       <c r="C107" s="47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D107" s="36">
         <v>0</v>
@@ -3939,29 +3936,35 @@
     </row>
     <row r="108" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="D108" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>228</v>
+        <v>227</v>
+      </c>
+      <c r="D109" s="33">
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B110" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C110" s="47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D110" s="36">
         <v>0</v>
@@ -3969,100 +3972,116 @@
     </row>
     <row r="111" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+      <c r="D111" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C112" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="D112" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C113" s="48" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C113" s="48" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" s="33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="44" t="s">
         <v>70</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+      <c r="D114" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="44" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="B115" s="44" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+      <c r="D115" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
         <v>121</v>
       </c>
       <c r="B116" s="44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C116" s="48" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B117" s="44" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C117" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="D117" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B118" s="44" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B118" s="44" t="s">
-        <v>142</v>
-      </c>
       <c r="C118" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="D118" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" s="43" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="B119" s="44" t="s">
-        <v>242</v>
-      </c>
-      <c r="C119" s="48" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B120" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="C120" s="48" t="s">
-        <v>244</v>
+      <c r="C119" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="D119" s="36">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4099,7 +4118,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4125,7 +4144,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D2" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -4143,12 +4162,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D5" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>64</v>
@@ -4156,7 +4175,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>61</v>
@@ -4164,28 +4183,20 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="32" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -4209,114 +4220,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>98</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="38" t="s">
         <v>100</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>103</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>106</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>110</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>116</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -4339,22 +4350,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -4364,7 +4375,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bar chart - section for period
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D7EA4B9-67E0-44DE-96B8-3927C8BEF144}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="1" r:id="rId1"/>
@@ -789,7 +790,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1209,7 +1210,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1492,32 +1493,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" style="29" customWidth="1"/>
     <col min="8" max="8" width="6" style="8" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="0.28515625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="8"/>
+    <col min="9" max="9" width="3.6640625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="0.33203125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>108.4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>21</v>
       </c>
@@ -1606,7 +1607,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>21</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
@@ -1682,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
       <c r="B7" s="11">
         <f t="shared" si="1"/>
@@ -1705,7 +1706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="11">
         <f t="shared" si="1"/>
@@ -1729,7 +1730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
@@ -1753,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
       <c r="B13" s="11">
         <f t="shared" si="1"/>
@@ -1849,7 +1850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="11">
         <f t="shared" si="1"/>
@@ -1873,7 +1874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="11">
         <f t="shared" si="1"/>
@@ -1891,7 +1892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="11">
         <f t="shared" si="1"/>
@@ -1909,7 +1910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
@@ -1937,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>21</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="11">
         <f t="shared" si="1"/>
@@ -1999,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
@@ -2021,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
@@ -2043,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="11">
         <f t="shared" si="1"/>
@@ -2061,7 +2062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="11">
         <f t="shared" si="1"/>
@@ -2077,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="11">
         <f t="shared" si="1"/>
@@ -2093,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="11">
         <f t="shared" si="1"/>
@@ -2115,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="15"/>
       <c r="B27" s="11">
         <f t="shared" si="1"/>
@@ -2137,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="15"/>
       <c r="B28" s="11">
         <f t="shared" si="1"/>
@@ -2159,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
       <c r="B29" s="11">
         <f t="shared" si="1"/>
@@ -2178,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
       <c r="B30" s="11">
         <f t="shared" si="1"/>
@@ -2197,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="11">
         <f t="shared" si="1"/>
@@ -2217,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A32" s="15"/>
       <c r="B32" s="11">
         <f t="shared" si="1"/>
@@ -2234,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="15"/>
       <c r="B33" s="11">
         <f t="shared" si="1"/>
@@ -2248,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="15"/>
       <c r="B34" s="11">
         <f t="shared" si="1"/>
@@ -2262,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="15"/>
       <c r="B35" s="11">
         <f t="shared" si="1"/>
@@ -2276,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="15"/>
       <c r="B36" s="11">
         <f t="shared" si="1"/>
@@ -2290,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="15"/>
       <c r="B37" s="11">
         <f t="shared" si="1"/>
@@ -2306,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
       <c r="B38" s="11">
         <f t="shared" si="1"/>
@@ -2320,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="15"/>
       <c r="B39" s="11">
         <f t="shared" si="1"/>
@@ -2334,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="15"/>
       <c r="B40" s="11">
         <f t="shared" si="1"/>
@@ -2348,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="B41" s="11">
         <f t="shared" si="1"/>
@@ -2362,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="11">
         <f t="shared" si="1"/>
@@ -2375,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="15"/>
       <c r="B43" s="11">
         <f t="shared" si="1"/>
@@ -2389,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="15"/>
       <c r="B44" s="11">
         <f t="shared" si="1"/>
@@ -2403,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="15"/>
       <c r="B45" s="11">
         <f t="shared" si="1"/>
@@ -2417,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
       <c r="B46" s="11">
         <f t="shared" si="1"/>
@@ -2431,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
       <c r="B47" s="11">
         <f t="shared" si="1"/>
@@ -2445,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="15"/>
       <c r="B48" s="11">
         <f t="shared" si="1"/>
@@ -2459,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="15"/>
       <c r="B49" s="11">
         <f t="shared" si="1"/>
@@ -2473,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="15"/>
       <c r="B50" s="11">
         <f t="shared" si="1"/>
@@ -2487,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
       <c r="B51" s="11">
         <f t="shared" si="1"/>
@@ -2501,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
       <c r="B52" s="11">
         <f t="shared" si="1"/>
@@ -2522,32 +2523,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="44" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="44" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" style="48" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="33" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="44" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="44" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="33" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="1.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" style="34" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="34" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="34" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" style="34" customWidth="1"/>
+    <col min="9" max="9" width="1.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.109375" style="34" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="34" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="34" customWidth="1"/>
+    <col min="13" max="13" width="26.5546875" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>117</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="51"/>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -2601,7 +2602,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>118</v>
       </c>
@@ -2620,7 +2621,7 @@
       <c r="J3" s="39"/>
       <c r="K3" s="39"/>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>119</v>
       </c>
@@ -2634,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
         <v>119</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
         <v>119</v>
       </c>
@@ -2662,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
         <v>119</v>
       </c>
@@ -2676,7 +2677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="43"/>
       <c r="B8" s="43" t="s">
         <v>148</v>
@@ -2688,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="43"/>
       <c r="B9" s="43" t="s">
         <v>148</v>
@@ -2700,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="43"/>
       <c r="B10" s="43" t="s">
         <v>148</v>
@@ -2712,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="43"/>
       <c r="B11" s="43" t="s">
         <v>148</v>
@@ -2724,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="43"/>
       <c r="B12" s="43" t="s">
         <v>148</v>
@@ -2736,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="43"/>
       <c r="B13" s="43" t="s">
         <v>148</v>
@@ -2748,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="43"/>
       <c r="B14" s="43" t="s">
         <v>140</v>
@@ -2760,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
         <v>119</v>
       </c>
@@ -2774,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="43"/>
       <c r="B16" s="43" t="s">
         <v>182</v>
@@ -2786,7 +2787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
         <v>119</v>
       </c>
@@ -2800,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>119</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="43"/>
       <c r="B19" s="43" t="s">
         <v>208</v>
@@ -2826,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
         <v>118</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="43" t="s">
         <v>118</v>
       </c>
@@ -2854,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
         <v>118</v>
       </c>
@@ -2868,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
         <v>119</v>
       </c>
@@ -2882,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="43"/>
       <c r="B24" s="43" t="s">
         <v>177</v>
@@ -2894,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="43" t="s">
         <v>118</v>
       </c>
@@ -2908,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="43" t="s">
         <v>119</v>
       </c>
@@ -2922,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="43" t="s">
         <v>119</v>
       </c>
@@ -2936,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>119</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
         <v>119</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="43"/>
       <c r="B30" s="43" t="s">
         <v>173</v>
@@ -2976,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="43"/>
       <c r="B31" s="43" t="s">
         <v>173</v>
@@ -2988,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="43"/>
       <c r="B32" s="43" t="s">
         <v>180</v>
@@ -3000,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="43" t="s">
         <v>119</v>
       </c>
@@ -3014,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="43" t="s">
         <v>118</v>
       </c>
@@ -3028,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="43" t="s">
         <v>118</v>
       </c>
@@ -3042,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>118</v>
       </c>
@@ -3056,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="43" t="s">
         <v>118</v>
       </c>
@@ -3070,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="43" t="s">
         <v>119</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
         <v>119</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="43" t="s">
         <v>119</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
         <v>119</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>119</v>
       </c>
@@ -3140,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
         <v>119</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
         <v>119</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="43" t="s">
         <v>119</v>
       </c>
@@ -3182,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="43" t="s">
         <v>119</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="43" t="s">
         <v>119</v>
       </c>
@@ -3210,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="43"/>
       <c r="B48" s="43" t="s">
         <v>169</v>
@@ -3222,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="43" t="s">
         <v>119</v>
       </c>
@@ -3236,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="43" t="s">
         <v>114</v>
       </c>
@@ -3250,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="43"/>
       <c r="B51" s="43" t="s">
         <v>127</v>
@@ -3262,7 +3263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="43"/>
       <c r="B52" s="43" t="s">
         <v>127</v>
@@ -3274,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="43"/>
       <c r="B53" s="43" t="s">
         <v>127</v>
@@ -3286,7 +3287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="43"/>
       <c r="B54" s="43" t="s">
         <v>127</v>
@@ -3298,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="43"/>
       <c r="B55" s="43" t="s">
         <v>127</v>
@@ -3310,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="43"/>
       <c r="B56" s="43" t="s">
         <v>127</v>
@@ -3322,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="43"/>
       <c r="B57" s="43" t="s">
         <v>127</v>
@@ -3334,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="43"/>
       <c r="B58" s="43" t="s">
         <v>127</v>
@@ -3346,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="43"/>
       <c r="B59" s="43" t="s">
         <v>127</v>
@@ -3358,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="43" t="s">
         <v>118</v>
       </c>
@@ -3372,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="43" t="s">
         <v>118</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="43" t="s">
         <v>118</v>
       </c>
@@ -3396,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="43" t="s">
         <v>118</v>
       </c>
@@ -3408,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="43" t="s">
         <v>118</v>
       </c>
@@ -3420,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="43" t="s">
         <v>69</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="43" t="s">
         <v>69</v>
       </c>
@@ -3444,7 +3445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="43" t="s">
         <v>69</v>
       </c>
@@ -3456,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="43" t="s">
         <v>69</v>
       </c>
@@ -3468,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="43" t="s">
         <v>69</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="43" t="s">
         <v>69</v>
       </c>
@@ -3492,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="43" t="s">
         <v>69</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="43" t="s">
         <v>69</v>
       </c>
@@ -3516,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="43" t="s">
         <v>69</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="43" t="s">
         <v>69</v>
       </c>
@@ -3540,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="43" t="s">
         <v>69</v>
       </c>
@@ -3552,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="43"/>
       <c r="B76" s="43"/>
       <c r="C76" s="47" t="s">
@@ -3562,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="44" t="s">
         <v>119</v>
       </c>
@@ -3576,7 +3577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="44" t="s">
         <v>69</v>
       </c>
@@ -3590,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="44" t="s">
         <v>119</v>
       </c>
@@ -3604,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="44" t="s">
         <v>119</v>
       </c>
@@ -3618,7 +3619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="44" t="s">
         <v>119</v>
       </c>
@@ -3632,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="44" t="s">
         <v>119</v>
       </c>
@@ -3646,7 +3647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="44" t="s">
         <v>119</v>
       </c>
@@ -3660,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="44" t="s">
         <v>119</v>
       </c>
@@ -3674,7 +3675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="44" t="s">
         <v>119</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="44" t="s">
         <v>118</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="44" t="s">
         <v>119</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="44" t="s">
         <v>118</v>
       </c>
@@ -3730,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="44" t="s">
         <v>118</v>
       </c>
@@ -3744,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="44" t="s">
         <v>119</v>
       </c>
@@ -3758,7 +3759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="44" t="s">
         <v>69</v>
       </c>
@@ -3772,7 +3773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="44" t="s">
         <v>69</v>
       </c>
@@ -3786,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="44" t="s">
         <v>69</v>
       </c>
@@ -3800,7 +3801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="44" t="s">
         <v>69</v>
       </c>
@@ -3814,7 +3815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="44" t="s">
         <v>119</v>
       </c>
@@ -3828,7 +3829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="44" t="s">
         <v>119</v>
       </c>
@@ -3842,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="44" t="s">
         <v>119</v>
       </c>
@@ -3856,7 +3857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="44" t="s">
         <v>119</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="44" t="s">
         <v>119</v>
       </c>
@@ -3884,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="44" t="s">
         <v>119</v>
       </c>
@@ -3898,7 +3899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="44" t="s">
         <v>69</v>
       </c>
@@ -3912,7 +3913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="44" t="s">
         <v>69</v>
       </c>
@@ -3926,7 +3927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="44" t="s">
         <v>69</v>
       </c>
@@ -3940,7 +3941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
         <v>118</v>
       </c>
@@ -3954,7 +3955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="44" t="s">
         <v>119</v>
       </c>
@@ -3968,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
         <v>119</v>
       </c>
@@ -3982,7 +3983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="44" t="s">
         <v>119</v>
       </c>
@@ -3996,7 +3997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="44" t="s">
         <v>119</v>
       </c>
@@ -4010,7 +4011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="44" t="s">
         <v>119</v>
       </c>
@@ -4024,7 +4025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="44" t="s">
         <v>118</v>
       </c>
@@ -4038,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="44" t="s">
         <v>119</v>
       </c>
@@ -4049,7 +4050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="44" t="s">
         <v>119</v>
       </c>
@@ -4060,7 +4061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="44" t="s">
         <v>119</v>
       </c>
@@ -4071,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="44" t="s">
         <v>119</v>
       </c>
@@ -4085,7 +4086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="44" t="s">
         <v>119</v>
       </c>
@@ -4099,7 +4100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
         <v>118</v>
       </c>
@@ -4113,7 +4114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="44" t="s">
         <v>69</v>
       </c>
@@ -4127,7 +4128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="44" t="s">
         <v>69</v>
       </c>
@@ -4141,7 +4142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="44" t="s">
         <v>119</v>
       </c>
@@ -4155,7 +4156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="44" t="s">
         <v>119</v>
       </c>
@@ -4169,7 +4170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="44" t="s">
         <v>114</v>
       </c>
@@ -4180,7 +4181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="44" t="s">
         <v>119</v>
       </c>
@@ -4194,7 +4195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="44" t="s">
         <v>119</v>
       </c>
@@ -4208,7 +4209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="44" t="s">
         <v>119</v>
       </c>
@@ -4219,7 +4220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="44" t="s">
         <v>119</v>
       </c>
@@ -4230,7 +4231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="44" t="s">
         <v>119</v>
       </c>
@@ -4238,7 +4239,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="44" t="s">
         <v>118</v>
       </c>
@@ -4269,7 +4270,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Help!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -4282,21 +4283,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" style="32" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" style="32" customWidth="1"/>
-    <col min="3" max="4" width="63.140625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" style="32" customWidth="1"/>
+    <col min="2" max="2" width="47.5546875" style="32" customWidth="1"/>
+    <col min="3" max="4" width="63.109375" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>72</v>
       </c>
@@ -4310,17 +4311,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D2" s="32" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" s="32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C4" s="32" t="s">
         <v>70</v>
       </c>
@@ -4328,12 +4329,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D5" s="32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="32" t="s">
         <v>82</v>
       </c>
@@ -4341,7 +4342,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="32" t="s">
         <v>84</v>
       </c>
@@ -4349,7 +4350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="32" t="s">
         <v>85</v>
       </c>
@@ -4357,12 +4358,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="32" t="s">
         <v>88</v>
       </c>
@@ -4373,20 +4374,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="38" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>96</v>
       </c>
@@ -4394,7 +4395,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>98</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>98</v>
       </c>
@@ -4410,7 +4411,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>101</v>
       </c>
@@ -4418,7 +4419,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>101</v>
       </c>
@@ -4426,7 +4427,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>104</v>
       </c>
@@ -4434,7 +4435,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>104</v>
       </c>
@@ -4442,7 +4443,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>107</v>
       </c>
@@ -4450,7 +4451,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>108</v>
       </c>
@@ -4458,7 +4459,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>99</v>
       </c>
@@ -4466,7 +4467,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>99</v>
       </c>
@@ -4474,7 +4475,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>108</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>99</v>
       </c>
@@ -4490,7 +4491,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
         <v>114</v>
       </c>
@@ -4504,44 +4505,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Update event state logic
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D7EA4B9-67E0-44DE-96B8-3927C8BEF144}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{62706DC1-578B-473B-8371-D64023D6E6C1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="258">
   <si>
     <t>№</t>
   </si>
@@ -688,9 +688,6 @@
     <t>Style refactoring</t>
   </si>
   <si>
-    <t>Make base class for track changes (like in DataFilter, PeriodFilter)</t>
-  </si>
-  <si>
     <t>Add tasks</t>
   </si>
   <si>
@@ -700,9 +697,6 @@
     <t>Insert calculator everywhere for enter amount</t>
   </si>
   <si>
-    <t>Action type is not refreshed after change</t>
-  </si>
-  <si>
     <t>Add defaults provider for new entities</t>
   </si>
   <si>
@@ -766,9 +760,6 @@
     <t>Build report with partitioning data by period</t>
   </si>
   <si>
-    <t>Build report for comparing incomes and expences</t>
-  </si>
-  <si>
     <t>Show events planned for today</t>
   </si>
   <si>
@@ -785,6 +776,33 @@
   </si>
   <si>
     <t>Translate all colors into russian</t>
+  </si>
+  <si>
+    <t>Show filter should not rebuild report</t>
+  </si>
+  <si>
+    <t>If "take current currency exchange rate" current exchange rate should be shown in details</t>
+  </si>
+  <si>
+    <t>Event details (record)</t>
+  </si>
+  <si>
+    <t>Event details (money transfer)</t>
+  </si>
+  <si>
+    <t>Category is not saved</t>
+  </si>
+  <si>
+    <t>Period selector</t>
+  </si>
+  <si>
+    <t>Custom period -&gt; cannot select more then one month</t>
+  </si>
+  <si>
+    <t>Create transaction from planned money transfer -&gt; if storage is hidden there is not selected storage in combobox</t>
+  </si>
+  <si>
+    <t>Event state is not refreshed after change</t>
   </si>
 </sst>
 </file>
@@ -2524,17 +2542,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
+      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="44" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="44" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" style="44" customWidth="1"/>
     <col min="3" max="3" width="48.6640625" style="48" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" style="33" customWidth="1"/>
     <col min="5" max="5" width="2.33203125" customWidth="1"/>
@@ -2584,22 +2602,22 @@
       <c r="D2" s="50"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43234</v>
+        <v>43254</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="J2" s="25">
-        <f>SUM(D3:D160)</f>
-        <v>88</v>
+        <f>SUM(D3:D157)</f>
+        <v>78</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-40</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2671,7 +2689,7 @@
         <v>148</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D7" s="36">
         <v>0</v>
@@ -3062,10 +3080,10 @@
         <v>118</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D37" s="36">
         <v>0</v>
@@ -3571,7 +3589,7 @@
         <v>148</v>
       </c>
       <c r="C77" s="48" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D77" s="33">
         <v>1</v>
@@ -3596,10 +3614,10 @@
         <v>119</v>
       </c>
       <c r="B79" s="44" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C79" s="48" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D79" s="33">
         <v>1</v>
@@ -3686,7 +3704,7 @@
         <v>213</v>
       </c>
       <c r="D85" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -3694,69 +3712,69 @@
         <v>118</v>
       </c>
       <c r="B86" s="44" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C86" s="48" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D86" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B87" s="44" t="s">
+      <c r="A87" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B87" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="C87" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="D87" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B88" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C88" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="D88" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A89" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C89" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="C87" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="D87" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B88" s="44" t="s">
+      <c r="D89" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B90" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="C88" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="D88" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B89" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="C89" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="D89" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="C90" s="48" t="s">
-        <v>226</v>
-      </c>
-      <c r="D90" s="33">
-        <v>1</v>
+      <c r="C90" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D90" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -3787,99 +3805,99 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="44" t="s">
         <v>69</v>
       </c>
       <c r="B93" s="44" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C93" s="48" t="s">
-        <v>219</v>
+        <v>73</v>
       </c>
       <c r="D93" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B94" s="44" t="s">
+      <c r="A94" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B94" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C94" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="D94" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A95" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B95" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C95" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="D95" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="C94" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="D94" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B95" s="44" t="s">
+      <c r="D96" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="C95" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="D95" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A96" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B96" s="44" t="s">
+      <c r="C97" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="D97" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="C96" s="48" t="s">
-        <v>241</v>
-      </c>
-      <c r="D96" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B97" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C97" s="48" t="s">
+      <c r="C98" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="D97" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B98" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C98" s="48" t="s">
-        <v>243</v>
-      </c>
-      <c r="D98" s="33">
-        <v>1</v>
+      <c r="D98" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B99" s="44" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="D99" s="33">
         <v>1</v>
@@ -3887,55 +3905,55 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B100" s="44" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="D100" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="44" t="s">
         <v>69</v>
       </c>
       <c r="B101" s="44" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>193</v>
+        <v>231</v>
       </c>
       <c r="D101" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B102" s="44" t="s">
-        <v>239</v>
-      </c>
-      <c r="C102" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="D102" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A102" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C102" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="D102" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="44" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="B103" s="44" t="s">
-        <v>250</v>
+        <v>169</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>233</v>
+        <v>170</v>
       </c>
       <c r="D103" s="33">
         <v>1</v>
@@ -3943,13 +3961,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B104" s="44" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>234</v>
+        <v>171</v>
       </c>
       <c r="D104" s="33">
         <v>1</v>
@@ -3963,7 +3981,7 @@
         <v>169</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="D105" s="33">
         <v>1</v>
@@ -3974,10 +3992,10 @@
         <v>119</v>
       </c>
       <c r="B106" s="44" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="D106" s="33">
         <v>1</v>
@@ -3988,10 +4006,10 @@
         <v>119</v>
       </c>
       <c r="B107" s="44" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>196</v>
+        <v>243</v>
       </c>
       <c r="D107" s="33">
         <v>1</v>
@@ -3999,13 +4017,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B108" s="44" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D108" s="33">
         <v>1</v>
@@ -4015,11 +4033,8 @@
       <c r="A109" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B109" s="44" t="s">
-        <v>127</v>
-      </c>
       <c r="C109" s="48" t="s">
-        <v>246</v>
+        <v>79</v>
       </c>
       <c r="D109" s="33">
         <v>1</v>
@@ -4027,13 +4042,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B110" s="44" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>238</v>
+        <v>190</v>
       </c>
       <c r="D110" s="33">
         <v>1</v>
@@ -4044,7 +4056,7 @@
         <v>119</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>79</v>
+        <v>217</v>
       </c>
       <c r="D111" s="33">
         <v>1</v>
@@ -4054,33 +4066,39 @@
       <c r="A112" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B112" s="44" t="s">
+        <v>157</v>
+      </c>
       <c r="C112" s="48" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="D112" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B113" s="44" t="s">
+        <v>157</v>
+      </c>
       <c r="C113" s="48" t="s">
-        <v>217</v>
+        <v>160</v>
       </c>
       <c r="D113" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B114" s="44" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>147</v>
+        <v>223</v>
       </c>
       <c r="D114" s="33">
         <v>2</v>
@@ -4088,13 +4106,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B115" s="44" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D115" s="33">
         <v>2</v>
@@ -4102,13 +4120,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="B116" s="44" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D116" s="33">
         <v>2</v>
@@ -4116,41 +4134,38 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="44" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="B117" s="44" t="s">
-        <v>240</v>
+        <v>157</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="D117" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="44" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="B118" s="44" t="s">
-        <v>239</v>
+        <v>157</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>232</v>
+        <v>164</v>
       </c>
       <c r="D118" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B119" s="44" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="D119" s="33">
         <v>3</v>
@@ -4161,52 +4176,49 @@
         <v>119</v>
       </c>
       <c r="B120" s="44" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D120" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="44" t="s">
-        <v>114</v>
+        <v>119</v>
+      </c>
+      <c r="B121" s="44" t="s">
+        <v>140</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>220</v>
+        <v>139</v>
       </c>
       <c r="D121" s="33">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B122" s="44" t="s">
-        <v>148</v>
-      </c>
       <c r="C122" s="48" t="s">
-        <v>152</v>
+        <v>15</v>
       </c>
       <c r="D122" s="33">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B123" s="44" t="s">
-        <v>140</v>
-      </c>
       <c r="C123" s="48" t="s">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="D123" s="33">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -4214,50 +4226,88 @@
         <v>119</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D124" s="33">
-        <v>10</v>
+        <v>221</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="B125" s="44" t="s">
+        <v>166</v>
       </c>
       <c r="C125" s="48" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="D125" s="33">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="C126" s="48" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B127" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="C127" s="48" t="s">
+      <c r="A126" s="43"/>
+      <c r="B126" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C126" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="D126" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A127" s="43"/>
+      <c r="B127" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="D127" s="33">
-        <v>1</v>
+      <c r="C127" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="D127" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="43"/>
+      <c r="B128" s="43" t="s">
+        <v>252</v>
+      </c>
+      <c r="C128" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="D128" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="43"/>
+      <c r="B129" s="43" t="s">
+        <v>254</v>
+      </c>
+      <c r="C129" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="D129" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A130" s="43"/>
+      <c r="B130" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="C130" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="D130" s="36">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:D126">
-    <sortCondition ref="D3:D126"/>
-    <sortCondition ref="B3:B126"/>
-    <sortCondition ref="A3:A126"/>
+  <sortState ref="A4:D124">
+    <sortCondition ref="D3:D124"/>
+    <sortCondition ref="B3:B124"/>
+    <sortCondition ref="A3:A124"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="C1:C2"/>

</xml_diff>

<commit_message>
Dashboard page -> today transactions
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{62706DC1-578B-473B-8371-D64023D6E6C1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AF2BB26E-6B12-48D7-8470-F5A476D2E8B8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2546,7 +2546,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
+      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,11 +2613,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-50</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2970,14 +2970,12 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="43" t="s">
-        <v>119</v>
-      </c>
+      <c r="A29" s="43"/>
       <c r="B29" s="43" t="s">
-        <v>173</v>
+        <v>252</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>206</v>
+        <v>253</v>
       </c>
       <c r="D29" s="36">
         <v>0</v>
@@ -2986,22 +2984,24 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="43"/>
       <c r="B30" s="43" t="s">
-        <v>173</v>
+        <v>251</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>172</v>
+        <v>250</v>
       </c>
       <c r="D30" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="43"/>
+      <c r="A31" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B31" s="43" t="s">
         <v>173</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="D31" s="36">
         <v>0</v>
@@ -3010,52 +3010,46 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="43"/>
       <c r="B32" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="43"/>
+      <c r="B33" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="43"/>
+      <c r="B34" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C34" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="D32" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>184</v>
-      </c>
       <c r="D34" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
-        <v>118</v>
-      </c>
+      <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
-        <v>128</v>
+        <v>254</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>185</v>
+        <v>255</v>
       </c>
       <c r="D35" s="36">
         <v>0</v>
@@ -3063,27 +3057,25 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>128</v>
+        <v>233</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="D36" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="43" t="s">
-        <v>118</v>
-      </c>
+      <c r="A37" s="43"/>
       <c r="B37" s="43" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
       <c r="D37" s="36">
         <v>0</v>
@@ -3091,13 +3083,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>129</v>
+        <v>257</v>
       </c>
       <c r="D38" s="36">
         <v>0</v>
@@ -3105,13 +3097,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>131</v>
+        <v>235</v>
       </c>
       <c r="D39" s="36">
         <v>0</v>
@@ -3122,10 +3114,10 @@
         <v>119</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C40" s="47" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D40" s="36">
         <v>0</v>
@@ -3136,10 +3128,10 @@
         <v>119</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>147</v>
+        <v>224</v>
       </c>
       <c r="D41" s="36">
         <v>0</v>
@@ -3147,13 +3139,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="C42" s="47" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="D42" s="36">
         <v>0</v>
@@ -3161,13 +3153,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="C43" s="47" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="D43" s="36">
         <v>0</v>
@@ -3175,13 +3167,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B44" s="43" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="C44" s="47" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="D44" s="36">
         <v>0</v>
@@ -3189,13 +3181,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>167</v>
+        <v>228</v>
       </c>
       <c r="D45" s="36">
         <v>0</v>
@@ -3206,10 +3198,10 @@
         <v>119</v>
       </c>
       <c r="B46" s="43" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D46" s="36">
         <v>0</v>
@@ -3220,22 +3212,24 @@
         <v>119</v>
       </c>
       <c r="B47" s="43" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
       <c r="D47" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="43"/>
+      <c r="A48" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B48" s="43" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="D48" s="36">
         <v>0</v>
@@ -3246,10 +3240,10 @@
         <v>119</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C49" s="47" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
       <c r="D49" s="36">
         <v>0</v>
@@ -3257,97 +3251,111 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="43" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B50" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>198</v>
+        <v>156</v>
       </c>
       <c r="D50" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="43"/>
+      <c r="A51" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B51" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C51" s="47" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="D51" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="43"/>
+      <c r="A52" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B52" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C52" s="47" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="D52" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="43"/>
+      <c r="A53" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B53" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C53" s="47" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="D53" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="43"/>
+      <c r="A54" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B54" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C54" s="47" t="s">
-        <v>130</v>
+        <v>239</v>
       </c>
       <c r="D54" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="43"/>
+      <c r="A55" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B55" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C55" s="47" t="s">
-        <v>131</v>
+        <v>240</v>
       </c>
       <c r="D55" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="43"/>
+      <c r="A56" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B56" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C56" s="47" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="D56" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="43"/>
+      <c r="A57" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B57" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C57" s="47" t="s">
-        <v>133</v>
+        <v>242</v>
       </c>
       <c r="D57" s="36">
         <v>0</v>
@@ -3356,22 +3364,24 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="43"/>
       <c r="B58" s="43" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C58" s="47" t="s">
-        <v>134</v>
+        <v>249</v>
       </c>
       <c r="D58" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="43"/>
+      <c r="A59" s="43" t="s">
+        <v>118</v>
+      </c>
       <c r="B59" s="43" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="C59" s="47" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="D59" s="36">
         <v>0</v>
@@ -3379,13 +3389,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="43" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B60" s="43" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C60" s="47" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="D60" s="36">
         <v>0</v>
@@ -3393,11 +3403,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B61" s="43"/>
+        <v>119</v>
+      </c>
+      <c r="B61" s="43" t="s">
+        <v>166</v>
+      </c>
       <c r="C61" s="47" t="s">
-        <v>66</v>
+        <v>165</v>
       </c>
       <c r="D61" s="36">
         <v>0</v>
@@ -3405,23 +3417,25 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B62" s="43"/>
+        <v>119</v>
+      </c>
+      <c r="B62" s="43" t="s">
+        <v>169</v>
+      </c>
       <c r="C62" s="47" t="s">
-        <v>94</v>
+        <v>195</v>
       </c>
       <c r="D62" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B63" s="43"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="43" t="s">
+        <v>169</v>
+      </c>
       <c r="C63" s="47" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="D63" s="36">
         <v>0</v>
@@ -3429,11 +3443,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B64" s="43"/>
+        <v>119</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C64" s="47" t="s">
-        <v>71</v>
+        <v>204</v>
       </c>
       <c r="D64" s="36">
         <v>0</v>
@@ -3441,119 +3457,121 @@
     </row>
     <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="43"/>
+        <v>114</v>
+      </c>
+      <c r="B65" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C65" s="47" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="D65" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="43"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C66" s="47" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D66" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="43"/>
+      <c r="A67" s="43"/>
+      <c r="B67" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C67" s="47" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="D67" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="43"/>
+      <c r="A68" s="43"/>
+      <c r="B68" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C68" s="47" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D68" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" s="43"/>
+      <c r="A69" s="43"/>
+      <c r="B69" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C69" s="47" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D69" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="43"/>
+      <c r="A70" s="43"/>
+      <c r="B70" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C70" s="47" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="D70" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B71" s="43"/>
+      <c r="A71" s="43"/>
+      <c r="B71" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C71" s="47" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="D71" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" s="43"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C72" s="47" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D72" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="43"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C73" s="47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D73" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B74" s="43"/>
+      <c r="A74" s="43"/>
+      <c r="B74" s="43" t="s">
+        <v>127</v>
+      </c>
       <c r="C74" s="47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D74" s="36">
         <v>0</v>
@@ -3561,175 +3579,157 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B75" s="43"/>
+        <v>118</v>
+      </c>
+      <c r="B75" s="43" t="s">
+        <v>191</v>
+      </c>
       <c r="C75" s="47" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="D75" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="43"/>
+      <c r="A76" s="43" t="s">
+        <v>118</v>
+      </c>
       <c r="B76" s="43"/>
       <c r="C76" s="47" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="D76" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B77" s="44" t="s">
-        <v>148</v>
-      </c>
-      <c r="C77" s="48" t="s">
-        <v>246</v>
-      </c>
-      <c r="D77" s="33">
-        <v>1</v>
+      <c r="A77" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="43"/>
+      <c r="C77" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="44" t="s">
+      <c r="A78" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="43"/>
+      <c r="C78" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="D78" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" s="43"/>
+      <c r="C79" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D79" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B78" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="C78" s="48" t="s">
-        <v>200</v>
-      </c>
-      <c r="D78" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B79" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="C79" s="48" t="s">
-        <v>229</v>
-      </c>
-      <c r="D79" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B80" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="C80" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="D80" s="33">
-        <v>1</v>
+      <c r="B80" s="43"/>
+      <c r="C80" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="D80" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B81" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="C81" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="D81" s="33">
-        <v>1</v>
+      <c r="A81" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" s="43"/>
+      <c r="C81" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D81" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B82" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="C82" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="D82" s="33">
-        <v>1</v>
+      <c r="A82" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B82" s="43"/>
+      <c r="C82" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="D82" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B83" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="C83" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="D83" s="33">
-        <v>1</v>
+      <c r="A83" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B83" s="43"/>
+      <c r="C83" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="D83" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B84" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="C84" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="D84" s="33">
-        <v>1</v>
+      <c r="A84" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" s="43"/>
+      <c r="C84" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="D84" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B85" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="C85" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="D85" s="33">
-        <v>3</v>
+      <c r="A85" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="43"/>
+      <c r="C85" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B86" s="44" t="s">
-        <v>244</v>
-      </c>
-      <c r="C86" s="48" t="s">
-        <v>245</v>
-      </c>
-      <c r="D86" s="33">
-        <v>1</v>
+      <c r="A86" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B86" s="43"/>
+      <c r="C86" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D86" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B87" s="43" t="s">
-        <v>233</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B87" s="43"/>
       <c r="C87" s="47" t="s">
-        <v>234</v>
+        <v>146</v>
       </c>
       <c r="D87" s="36">
         <v>0</v>
@@ -3737,13 +3737,11 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B88" s="43" t="s">
-        <v>124</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B88" s="43"/>
       <c r="C88" s="47" t="s">
-        <v>257</v>
+        <v>136</v>
       </c>
       <c r="D88" s="36">
         <v>0</v>
@@ -3751,13 +3749,11 @@
     </row>
     <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B89" s="43" t="s">
-        <v>124</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B89" s="43"/>
       <c r="C89" s="47" t="s">
-        <v>235</v>
+        <v>137</v>
       </c>
       <c r="D89" s="36">
         <v>0</v>
@@ -3765,41 +3761,35 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" s="43" t="s">
-        <v>124</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B90" s="43"/>
       <c r="C90" s="47" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D90" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B91" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="C91" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="D91" s="33">
-        <v>1</v>
+      <c r="A91" s="43"/>
+      <c r="B91" s="43"/>
+      <c r="C91" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D91" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="44" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="B92" s="44" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="C92" s="48" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="D92" s="33">
         <v>1</v>
@@ -3810,94 +3800,94 @@
         <v>69</v>
       </c>
       <c r="B93" s="44" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="C93" s="48" t="s">
-        <v>73</v>
+        <v>200</v>
       </c>
       <c r="D93" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B94" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C94" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="D94" s="36">
-        <v>0</v>
+      <c r="A94" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B94" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C94" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="D94" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A95" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B95" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C95" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="D95" s="36">
-        <v>0</v>
+      <c r="A95" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B95" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C95" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="D95" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B96" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C96" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="D96" s="36">
-        <v>0</v>
+      <c r="A96" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C96" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="D96" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B97" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C97" s="47" t="s">
-        <v>241</v>
-      </c>
-      <c r="D97" s="36">
-        <v>0</v>
+      <c r="A97" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C97" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="D97" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="B98" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C98" s="47" t="s">
-        <v>242</v>
-      </c>
-      <c r="D98" s="36">
-        <v>0</v>
+      <c r="A98" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C98" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="D98" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="44" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="B99" s="44" t="s">
-        <v>237</v>
+        <v>175</v>
       </c>
       <c r="C99" s="48" t="s">
-        <v>193</v>
+        <v>216</v>
       </c>
       <c r="D99" s="33">
         <v>1</v>
@@ -3905,13 +3895,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="44" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="B100" s="44" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C100" s="48" t="s">
-        <v>222</v>
+        <v>245</v>
       </c>
       <c r="D100" s="33">
         <v>1</v>
@@ -3922,38 +3912,38 @@
         <v>69</v>
       </c>
       <c r="B101" s="44" t="s">
-        <v>247</v>
+        <v>69</v>
       </c>
       <c r="C101" s="48" t="s">
-        <v>231</v>
+        <v>81</v>
       </c>
       <c r="D101" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B102" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="C102" s="47" t="s">
-        <v>232</v>
-      </c>
-      <c r="D102" s="36">
-        <v>0</v>
+      <c r="A102" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B102" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C102" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="D102" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B103" s="44" t="s">
-        <v>169</v>
+        <v>238</v>
       </c>
       <c r="C103" s="48" t="s">
-        <v>170</v>
+        <v>73</v>
       </c>
       <c r="D103" s="33">
         <v>1</v>
@@ -3961,13 +3951,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B104" s="44" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="C104" s="48" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="D104" s="33">
         <v>1</v>
@@ -3975,13 +3965,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B105" s="44" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="C105" s="48" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="D105" s="33">
         <v>1</v>
@@ -3989,13 +3979,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B106" s="44" t="s">
-        <v>127</v>
+        <v>247</v>
       </c>
       <c r="C106" s="48" t="s">
-        <v>80</v>
+        <v>231</v>
       </c>
       <c r="D106" s="33">
         <v>1</v>
@@ -4003,13 +3993,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B107" s="44" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="C107" s="48" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D107" s="33">
         <v>1</v>
@@ -4017,13 +4007,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B108" s="44" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
       <c r="D108" s="33">
         <v>1</v>
@@ -4033,8 +4023,11 @@
       <c r="A109" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B109" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="C109" s="48" t="s">
-        <v>79</v>
+        <v>171</v>
       </c>
       <c r="D109" s="33">
         <v>1</v>
@@ -4044,8 +4037,11 @@
       <c r="A110" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B110" s="44" t="s">
+        <v>169</v>
+      </c>
       <c r="C110" s="48" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D110" s="33">
         <v>1</v>
@@ -4055,8 +4051,11 @@
       <c r="A111" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B111" s="44" t="s">
+        <v>127</v>
+      </c>
       <c r="C111" s="48" t="s">
-        <v>217</v>
+        <v>80</v>
       </c>
       <c r="D111" s="33">
         <v>1</v>
@@ -4067,52 +4066,46 @@
         <v>119</v>
       </c>
       <c r="B112" s="44" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>147</v>
+        <v>243</v>
       </c>
       <c r="D112" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B113" s="44" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>160</v>
+        <v>236</v>
       </c>
       <c r="D113" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B114" s="44" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>223</v>
+        <v>79</v>
       </c>
       <c r="D114" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B115" s="44" t="s">
-        <v>238</v>
+        <v>119</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="D115" s="33">
         <v>2</v>
@@ -4120,16 +4113,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B116" s="44" t="s">
-        <v>237</v>
+        <v>119</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="D116" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -4140,10 +4130,10 @@
         <v>157</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D117" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -4154,160 +4144,170 @@
         <v>157</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D118" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="44" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="B119" s="44" t="s">
+        <v>123</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D119" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B120" s="44" t="s">
-        <v>148</v>
+        <v>238</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D120" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="44" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B121" s="44" t="s">
-        <v>140</v>
+        <v>237</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>139</v>
+        <v>230</v>
       </c>
       <c r="D121" s="33">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B122" s="44" t="s">
+        <v>157</v>
+      </c>
       <c r="C122" s="48" t="s">
-        <v>15</v>
+        <v>158</v>
       </c>
       <c r="D122" s="33">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B123" s="44" t="s">
+        <v>157</v>
+      </c>
       <c r="C123" s="48" t="s">
-        <v>225</v>
+        <v>164</v>
       </c>
       <c r="D123" s="33">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="44" t="s">
         <v>119</v>
       </c>
+      <c r="B124" s="44" t="s">
+        <v>107</v>
+      </c>
       <c r="C124" s="48" t="s">
-        <v>221</v>
+        <v>213</v>
+      </c>
+      <c r="D124" s="33">
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B125" s="44" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="C125" s="48" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="D125" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="43"/>
-      <c r="B126" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C126" s="47" t="s">
-        <v>249</v>
-      </c>
-      <c r="D126" s="36">
-        <v>0</v>
+      <c r="A126" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B126" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C126" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="D126" s="33">
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A127" s="43"/>
-      <c r="B127" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="C127" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="D127" s="36">
-        <v>0</v>
+      <c r="A127" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B127" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C127" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="D127" s="33">
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="43"/>
-      <c r="B128" s="43" t="s">
-        <v>252</v>
-      </c>
-      <c r="C128" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="D128" s="36">
-        <v>0</v>
+      <c r="A128" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C128" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" s="33">
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="43"/>
-      <c r="B129" s="43" t="s">
-        <v>254</v>
-      </c>
-      <c r="C129" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="D129" s="36">
-        <v>0</v>
+      <c r="A129" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="D129" s="33">
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A130" s="43"/>
-      <c r="B130" s="43" t="s">
-        <v>233</v>
-      </c>
-      <c r="C130" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="D130" s="36">
-        <v>0</v>
+      <c r="A130" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C130" s="48" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:D124">
-    <sortCondition ref="D3:D124"/>
-    <sortCondition ref="B3:B124"/>
-    <sortCondition ref="A3:A124"/>
+  <sortState ref="A4:D130">
+    <sortCondition ref="D3:D130"/>
+    <sortCondition ref="B3:B130"/>
+    <sortCondition ref="A3:A130"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="C1:C2"/>

</xml_diff>

<commit_message>
Planned for today transactions
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AF2BB26E-6B12-48D7-8470-F5A476D2E8B8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="266">
   <si>
     <t>№</t>
   </si>
@@ -803,12 +802,36 @@
   </si>
   <si>
     <t>Event state is not refreshed after change</t>
+  </si>
+  <si>
+    <t>Cannot select empty category in category details</t>
+  </si>
+  <si>
+    <t>Category details</t>
+  </si>
+  <si>
+    <t>Show planned transactions</t>
+  </si>
+  <si>
+    <t>Dublicate -&gt; resultat amount without currency</t>
+  </si>
+  <si>
+    <t>Select new category</t>
+  </si>
+  <si>
+    <t>Filter templates (for reports)</t>
+  </si>
+  <si>
+    <t>Transactions list</t>
+  </si>
+  <si>
+    <t>Update date record to last month -&gt; exception</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1511,7 +1534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:L52"/>
   <sheetViews>
@@ -2541,12 +2564,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M130"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
+      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2602,22 +2625,22 @@
       <c r="D2" s="50"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43254</v>
+        <v>43283</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>28</v>
+        <v>-1</v>
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-51</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2981,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="43"/>
       <c r="B30" s="43" t="s">
         <v>251</v>
@@ -3031,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="43"/>
       <c r="B34" s="43" t="s">
         <v>180</v>
@@ -3055,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>119</v>
       </c>
@@ -3069,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="43"/>
       <c r="B37" s="43" t="s">
         <v>233</v>
@@ -3095,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
         <v>118</v>
       </c>
@@ -3137,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>118</v>
       </c>
@@ -3305,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="43" t="s">
         <v>119</v>
       </c>
@@ -3455,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="43" t="s">
         <v>114</v>
       </c>
@@ -3541,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="43"/>
       <c r="B72" s="43" t="s">
         <v>127</v>
@@ -3591,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="43" t="s">
         <v>118</v>
       </c>
@@ -3639,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="43" t="s">
         <v>69</v>
       </c>
@@ -3747,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="43" t="s">
         <v>69</v>
       </c>
@@ -3771,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="43"/>
       <c r="B91" s="43"/>
       <c r="C91" s="47" t="s">
@@ -3823,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="44" t="s">
         <v>119</v>
       </c>
@@ -3852,17 +3875,17 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B97" s="44" t="s">
+      <c r="A97" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="C97" s="48" t="s">
+      <c r="C97" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="D97" s="33">
-        <v>1</v>
+      <c r="D97" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -3907,7 +3930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="44" t="s">
         <v>69</v>
       </c>
@@ -3977,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
         <v>69</v>
       </c>
@@ -4123,17 +4146,17 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B117" s="44" t="s">
+      <c r="A117" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="C117" s="48" t="s">
+      <c r="C117" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="D117" s="33">
-        <v>2</v>
+      <c r="D117" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -4242,7 +4265,7 @@
         <v>219</v>
       </c>
       <c r="D125" s="33">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -4259,7 +4282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="44" t="s">
         <v>119</v>
       </c>
@@ -4295,12 +4318,82 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="44" t="s">
         <v>119</v>
       </c>
       <c r="C130" s="48" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B131" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C131" s="48" t="s">
+        <v>258</v>
+      </c>
+      <c r="D131" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B132" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="C132" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="D132" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B133" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C133" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="D133" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B134" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="C134" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="D134" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B135" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="C135" s="48" t="s">
+        <v>265</v>
+      </c>
+      <c r="D135" s="33">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4320,7 +4413,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -4333,11 +4426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4408,6 +4501,11 @@
         <v>95</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="32" t="s">
+        <v>263</v>
+      </c>
+    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="32" t="s">
         <v>87</v>
@@ -4424,7 +4522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4555,7 +4653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Dashboard panel - Planned transactions from selected date until today
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1539,7 +1539,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -2568,8 +2568,8 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
+      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2625,22 +2625,22 @@
       <c r="D2" s="50"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43283</v>
+        <v>43645</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>-1</v>
+        <v>-363</v>
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-85</v>
+        <v>-445</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4160,17 +4160,17 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B118" s="44" t="s">
+      <c r="A118" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B118" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="C118" s="48" t="s">
+      <c r="C118" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="D118" s="33">
-        <v>2</v>
+      <c r="D118" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Minor dashboard items fixes
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -2568,8 +2568,8 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
+      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2625,22 +2625,22 @@
       <c r="D2" s="50"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43645</v>
+        <v>43646</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>-363</v>
+        <v>-364</v>
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-445</v>
+        <v>-443</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3861,17 +3861,17 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B96" s="44" t="s">
+      <c r="A96" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="C96" s="48" t="s">
+      <c r="C96" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="D96" s="33">
-        <v>1</v>
+      <c r="D96" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -4124,14 +4124,15 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="C115" s="48" t="s">
+      <c r="A115" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B115" s="43"/>
+      <c r="C115" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="D115" s="33">
-        <v>2</v>
+      <c r="D115" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix transaction replacement exception
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -2597,8 +2597,8 @@
   <dimension ref="A1:M137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
+      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2665,11 +2665,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-446</v>
+        <v>-444</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4399,31 +4399,31 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="49" t="s">
+      <c r="A134" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="B134" s="49" t="s">
+      <c r="B134" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="C134" s="50" t="s">
+      <c r="C134" s="47" t="s">
         <v>262</v>
       </c>
-      <c r="D134" s="51">
-        <v>1</v>
+      <c r="D134" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="49" t="s">
+      <c r="A135" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="B135" s="49" t="s">
+      <c r="B135" s="43" t="s">
         <v>264</v>
       </c>
-      <c r="C135" s="50" t="s">
+      <c r="C135" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="D135" s="51">
-        <v>1</v>
+      <c r="D135" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Show result value in different currencies
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="272">
   <si>
     <t>№</t>
   </si>
@@ -838,6 +838,12 @@
   </si>
   <si>
     <t>When event was paused and now is active, cannot pause it again</t>
+  </si>
+  <si>
+    <t>Templates</t>
+  </si>
+  <si>
+    <t>Transactions</t>
   </si>
 </sst>
 </file>
@@ -2594,11 +2600,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M137"/>
+  <dimension ref="A1:M138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
+      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2654,22 +2660,22 @@
       <c r="D2" s="53"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43647</v>
+        <v>43651</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>-365</v>
+        <v>-369</v>
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-444</v>
+        <v>-451</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4452,6 +4458,20 @@
       </c>
       <c r="D137" s="51">
         <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B138" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="C138" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="D138" s="51">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reports page - planned transactions
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="272">
   <si>
     <t>№</t>
   </si>
@@ -2603,8 +2603,8 @@
   <dimension ref="A1:M138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
+      <pane ySplit="2" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2660,22 +2660,22 @@
       <c r="D2" s="53"/>
       <c r="F2" s="27">
         <f ca="1">TODAY()</f>
-        <v>43651</v>
+        <v>43736</v>
       </c>
       <c r="G2" s="27">
         <v>43282</v>
       </c>
       <c r="H2" s="25">
         <f ca="1">G2-F2</f>
-        <v>-369</v>
+        <v>-454</v>
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-451</v>
+        <v>-531</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3830,7 +3830,9 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A91" s="43"/>
+      <c r="A91" s="43" t="s">
+        <v>119</v>
+      </c>
       <c r="B91" s="43"/>
       <c r="C91" s="47" t="s">
         <v>113</v>
@@ -4377,17 +4379,17 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B132" s="44" t="s">
+      <c r="A132" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B132" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="C132" s="48" t="s">
+      <c r="C132" s="47" t="s">
         <v>260</v>
       </c>
-      <c r="D132" s="33">
-        <v>2</v>
+      <c r="D132" s="36">
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -4461,17 +4463,17 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="B138" s="49" t="s">
+      <c r="A138" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B138" s="43" t="s">
         <v>271</v>
       </c>
-      <c r="C138" s="50" t="s">
+      <c r="C138" s="47" t="s">
         <v>270</v>
       </c>
-      <c r="D138" s="51">
-        <v>3</v>
+      <c r="D138" s="36">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4508,7 +4510,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4604,7 +4606,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Limits & Debts & DataFilter - updates
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="275">
   <si>
     <t>№</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>PaymentType changing don't work correct if saved is DifferentialPayment</t>
+  </si>
+  <si>
+    <t>Opposite rate</t>
   </si>
 </sst>
 </file>
@@ -2606,11 +2609,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M139"/>
+  <dimension ref="A1:M140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C149" sqref="C149"/>
+      <pane ySplit="2" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,11 +2680,11 @@
       </c>
       <c r="J2" s="25">
         <f>SUM(D3:D157)</f>
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K2" s="25">
         <f ca="1">H2-J2</f>
-        <v>-533</v>
+        <v>-535</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4494,6 +4497,20 @@
       </c>
       <c r="D139" s="33">
         <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B140" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C140" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="D140" s="33">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>